<commit_message>
minor adjustments to multipliers
</commit_message>
<xml_diff>
--- a/Stocks_fundamentals.xlsx
+++ b/Stocks_fundamentals.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/935cc860ba0efd68/GitHub/equity_research/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{46F93A60-A761-4650-86FD-7E9C13053220}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="89" documentId="8_{46F93A60-A761-4650-86FD-7E9C13053220}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{4D0B01A5-547A-49B1-A1C6-A155418E580F}"/>
   <bookViews>
-    <workbookView xWindow="57480" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12432" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Overview" sheetId="1" r:id="rId1"/>
@@ -104,7 +104,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="158" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="166" uniqueCount="63">
   <si>
     <t>Company</t>
   </si>
@@ -270,17 +270,42 @@
   <si>
     <t>Book Value per share (in Bil)</t>
   </si>
+  <si>
+    <t>ROE</t>
+  </si>
+  <si>
+    <t>ROIC</t>
+  </si>
+  <si>
+    <t>Reinvestment rate (capex ratio)</t>
+  </si>
+  <si>
+    <t>Book Value (total equity)</t>
+  </si>
+  <si>
+    <t>BPER</t>
+  </si>
+  <si>
+    <t>BUZZI</t>
+  </si>
+  <si>
+    <t>NVIDIA</t>
+  </si>
+  <si>
+    <t>AMAZON</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="5">
-    <numFmt numFmtId="168" formatCode="_([$$-409]* #,##0_);_([$$-409]* \(#,##0\);_([$$-409]* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="169" formatCode="_([$€-2]\ * #,##0_);_([$€-2]\ * \(#,##0\);_([$€-2]\ * &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="171" formatCode="0.0"/>
-    <numFmt numFmtId="186" formatCode="_([$$-409]* #,##0.00_);_([$$-409]* \(#,##0.00\);_([$$-409]* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="189" formatCode="_([$€-2]\ * #,##0.00_);_([$€-2]\ * \(#,##0.00\);_([$€-2]\ * &quot;-&quot;_);_(@_)"/>
+  <numFmts count="6">
+    <numFmt numFmtId="164" formatCode="_([$$-409]* #,##0_);_([$$-409]* \(#,##0\);_([$$-409]* &quot;-&quot;_);_(@_)"/>
+    <numFmt numFmtId="165" formatCode="_([$€-2]\ * #,##0_);_([$€-2]\ * \(#,##0\);_([$€-2]\ * &quot;-&quot;_);_(@_)"/>
+    <numFmt numFmtId="166" formatCode="0.0"/>
+    <numFmt numFmtId="167" formatCode="_([$$-409]* #,##0.00_);_([$$-409]* \(#,##0.00\);_([$$-409]* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="168" formatCode="_([$€-2]\ * #,##0.00_);_([$€-2]\ * \(#,##0.00\);_([$€-2]\ * &quot;-&quot;_);_(@_)"/>
+    <numFmt numFmtId="170" formatCode="0.0%"/>
   </numFmts>
   <fonts count="8" x14ac:knownFonts="1">
     <font>
@@ -363,7 +388,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -386,12 +411,34 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="33">
+  <cellXfs count="40">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
@@ -432,17 +479,16 @@
     <xf numFmtId="17" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="2" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
@@ -453,7 +499,7 @@
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="171" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="10" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
@@ -462,12 +508,32 @@
     <xf numFmtId="10" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="171" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="186" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="189" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="170" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -616,28 +682,25 @@
     <v>Finance</v>
     <v>5</v>
     <v>1996</v>
-    <v>204.84</v>
+    <v>204.98</v>
     <v>10616350000</v>
     <v>1.3393999999999999</v>
-    <v>-1.756E-3</v>
-    <v>-0.36</v>
     <v>2176459000000</v>
-    <v>205.7</v>
+    <v>205.01</v>
     <v>Amazon.com, Inc. Fornisce una gamma di prodotti e servizi ai clienti. I prodotti offerti attraverso i suoi punti vendita includono prodotti e contenuti acquistati per la rivendita e prodotti offerti da venditori terzi. I segmenti della società comprendono Nord America, International e Amazon Web Services (AWS). Serve i consumatori attraverso i suoi negozi online e fisici e si concentra sulla selezione, il prezzo e la convenienza. I clienti accedono alle proprie offerte tramite i propri siti Web, app mobili, Alexa, dispositivi, streaming, e visitando fisicamente i suoi negozi. Produce e vende anche dispositivi elettronici, tra cui Kindle, Fire tablet, Fire TV, Echo, ring, Blink ed eero, e sviluppa e produce contenuti multimediali. Serve sviluppatori e imprese di tutte le dimensioni, comprese Start-up, agenzie governative e istituzioni accademiche, tramite AWS, che offre una serie di servizi tecnologici on-demand, tra cui elaborazione, storage, database, analisi, e l'apprendimento automatico e altri servizi.</v>
     <v>1560000</v>
     <v>Nasdaq Stock Market</v>
     <v>XNAS</v>
     <v>0</v>
-    <v>205.99</v>
+    <v>206.92</v>
     <v>242.52</v>
-    <v>201.69499999999999</v>
+    <v>202.68</v>
     <v>151.61000000000001</v>
     <v>AMAZON.COM, INC.</v>
     <v>AMAZON.COM, INC.</v>
-    <v>45807.999999212501</v>
-    <v>33.547499999999999</v>
-    <v>205.01</v>
-    <v>204.65</v>
+    <v>45810.813003495314</v>
+    <v>33.736199999999997</v>
+    <v>206.85679999999999</v>
     <v>410 Terry Avenue North, SEATTLE, WA, 98109 US</v>
     <v>Diversified Retail</v>
     <v>XNAS</v>
@@ -645,10 +708,10 @@
     <v>Azionario</v>
     <v>AMAZON.COM, INC. (XNAS:AMZN)</v>
     <v>USD</v>
-    <v>-0.69</v>
-    <v>-3.3539999999999998E-3</v>
-    <v>51679406</v>
-    <v>43837348</v>
+    <v>1.8468</v>
+    <v>9.0080000000000004E-3</v>
+    <v>21534643</v>
+    <v>44153996</v>
   </rv>
   <rv s="2">
     <v>1</v>
@@ -670,25 +733,25 @@
     <v>8</v>
     <v>Finance</v>
     <v>9</v>
-    <v>7.7619999999999996</v>
+    <v>7.8239999999999998</v>
     <v>1421624000</v>
     <v>1.5492999999999999</v>
     <v>11105730000</v>
-    <v>7.7380000000000004</v>
+    <v>7.8120000000000003</v>
     <v>BPER BANCA S.P.A., già Banca Popolare dell'Emilia Romagna Società cooperativa, è un gruppo bancario italiano con sede in Italia, che offre servizi bancari tradizionali a privati, società, liberi professionisti ed enti pubblici. I suoi servizi bancari sono divisi in sette segmenti. Il segmento Private serve conti individuali e cointestati. Il segmento Retail si rivolge a ditte individuali, associazioni e società a responsabilità limitata, tra gli altri. Il segmento Corporate comprende la pubblica amministrazione, nonché società non finanziarie e non residenti. Il segmento Large Corporate copre i servizi bancari con clienti aziendali e associazioni. Il segmento Finance copre le attività di tesoreria e la gestione del portafoglio d‘investimento del Gruppo. Il segmento Corporate Center copre attività connesse alla governance del Gruppo, alle decisioni strategiche e ai relativi risultati, nonché attività non direttamente connesse ad altre aree dell‘impresa. La divisione Altre attività comprende i risultati delle società non bancarie del Gruppo.</v>
     <v>19231</v>
     <v>Borsa Italiana</v>
     <v>XMIL</v>
     <v>3</v>
-    <v>7.8140000000000001</v>
+    <v>7.8680000000000003</v>
     <v>8.0500000000000007</v>
-    <v>7.7220000000000004</v>
+    <v>7.6619999999999999</v>
     <v>4.26</v>
     <v>BPER BANCA S.P.A.</v>
     <v>BPER BANCA S.P.A.</v>
-    <v>45807.666666666664</v>
-    <v>7.9016000000000002</v>
-    <v>7.8120000000000003</v>
+    <v>45810.666666666664</v>
+    <v>7.9771000000000001</v>
+    <v>7.7480000000000002</v>
     <v>Via San Carlo, 8/20, MODENA, MODENA, 41121 IT</v>
     <v>Banking Services</v>
     <v>XMIL</v>
@@ -696,9 +759,9 @@
     <v>Azionario</v>
     <v>BPER BANCA S.P.A. (XMIL:BPE)</v>
     <v>EUR</v>
-    <v>7.3999999999999996E-2</v>
-    <v>9.5630000000000003E-3</v>
-    <v>14162321</v>
+    <v>-6.4000000000000001E-2</v>
+    <v>-8.1930000000000006E-3</v>
+    <v>7768209</v>
     <v>13771580</v>
   </rv>
   <rv s="2">
@@ -721,25 +784,25 @@
     <v>10</v>
     <v>Finance</v>
     <v>11</v>
-    <v>25.6</v>
+    <v>25.355</v>
     <v>192626100</v>
     <v>0.9274</v>
     <v>8710555000</v>
-    <v>26.46</v>
+    <v>25.85</v>
     <v>Buzzi Spa, precedentemente nota come Buzzi Unicem Spa, è una società con sede in Italia impegnata nella produzione di materiali da costruzione. L'azienda opera principalmente nella produzione, distribuzione e vendita di cemento, calcestruzzo pronto all'uso e aggregati naturali. Le attività della società sono ubicate in Italia, Stati Uniti, Germania, Lussemburgo e Paesi Bassi, Polonia, Repubblica ceca e Slovacchia, Ucraina, Russia, Messico, Brasile, e l'Algeria. Le tre principali aree geografiche con la maggiore generazione di entrate sono: Stati Uniti, Germania e Messico. L'azienda è inoltre impegnata nell'attività di ricerca e sviluppo con l'obiettivo di sviluppare e sperimentare innovazioni da utilizzare nella filiera produttiva e per i propri prodotti. Questa attività viene svolta in collaborazione con centri di ricerca nazionali, università e laboratori privati.</v>
     <v>10061</v>
     <v>OTC Markets</v>
     <v>OTCM</v>
     <v>6</v>
-    <v>25.85</v>
+    <v>25.63</v>
     <v>29.487500000000001</v>
-    <v>25.5</v>
+    <v>25.355</v>
     <v>17.649999999999999</v>
     <v>Buzzi SpA</v>
     <v>Buzzi SpA</v>
-    <v>45807.788522372655</v>
+    <v>45810.790938171092</v>
     <v>0</v>
-    <v>25.85</v>
+    <v>25.63</v>
     <v>Via Luigi Buzzi, 6, CASALE MONFERRATO, ALESSANDRIA, 15033 IT</v>
     <v>Construction Materials</v>
     <v>OTCM</v>
@@ -747,9 +810,9 @@
     <v>Azionario</v>
     <v>Buzzi SpA (OTCM:BZZUY)</v>
     <v>USD</v>
-    <v>-0.61</v>
-    <v>-2.3054000000000002E-2</v>
-    <v>6632</v>
+    <v>-0.22</v>
+    <v>-8.5109999999999995E-3</v>
+    <v>4672</v>
     <v>288300</v>
   </rv>
   <rv s="2">
@@ -773,28 +836,25 @@
     <v>Finance</v>
     <v>5</v>
     <v>1998</v>
-    <v>138.715</v>
+    <v>135.5</v>
     <v>24400000000</v>
     <v>2.1208999999999998</v>
-    <v>-4.5140000000000007E-3</v>
-    <v>-0.61</v>
-    <v>3297172000000</v>
-    <v>139.19</v>
+    <v>3357269199999</v>
+    <v>135.13</v>
     <v>NVIDIA Corporation è un'azienda di infrastrutture informatiche full-stack. L'azienda è impegnata nel computing accelerato per aiutare a risolvere i problemi computazionali più complessi. I segmenti dell'azienda includono computing, networking e grafica. Il segmento Compute &amp; Networking include le sue piattaforme informatiche accelerate per data center e soluzioni e software di intelligenza artificiale (ai); networking; piattaforme automobilistiche e soluzioni per veicoli elettrici ed autonomi; Jetson per robotica e altre piattaforme embedded e servizi di cloud computing DGX. Il segmento della grafica include GPU GeForce per giochi e PC, il servizio di streaming di giochi GeForce e la relativa infrastruttura, e soluzioni per piattaforme di gioco; GPU quadro/NVIDIA RTX per la grafica di workstation aziendali; software GPU virtuale per il computing virtuale e visivo basato su cloud; piattaforme automobilistiche per sistemi di infotainment e software Omniverse Enterprise per la costruzione e il funzionamento di IA industriale e applicazioni gemelle digitali.</v>
     <v>36000</v>
     <v>Nasdaq Stock Market</v>
     <v>XNAS</v>
     <v>9</v>
-    <v>139.62</v>
+    <v>138.12</v>
     <v>153.13</v>
-    <v>132.91999999999999</v>
+    <v>135.41999999999999</v>
     <v>86.62</v>
     <v>NVIDIA CORPORATION</v>
     <v>NVIDIA CORPORATION</v>
-    <v>45807.999990937496</v>
-    <v>44.835099999999997</v>
-    <v>135.13</v>
-    <v>134.52000000000001</v>
+    <v>45810.813025010939</v>
+    <v>44.320500000000003</v>
+    <v>137.59299999999999</v>
     <v>2788 San Tomas Expressway, SANTA CLARA, CA, 95051 US</v>
     <v>Semiconductors &amp; Semiconductor Equipment</v>
     <v>XNAS</v>
@@ -802,10 +862,10 @@
     <v>Azionario</v>
     <v>NVIDIA CORPORATION (XNAS:NVDA)</v>
     <v>USD</v>
-    <v>-4.0599999999999996</v>
-    <v>-2.9169E-2</v>
-    <v>333170851</v>
-    <v>220446096</v>
+    <v>2.4630000000000001</v>
+    <v>1.8227E-2</v>
+    <v>147280209</v>
+    <v>224940328</v>
   </rv>
   <rv s="2">
     <v>10</v>
@@ -836,8 +896,6 @@
     <k n="Apri"/>
     <k n="Azioni in circolazione"/>
     <k n="Beta"/>
-    <k n="Cambia % (orario prolungato)"/>
-    <k n="Cambia (orario prolungato)"/>
     <k n="Capitalizzazione di mercato"/>
     <k n="Chiusura precedente"/>
     <k n="Descrizione" t="s"/>
@@ -854,7 +912,6 @@
     <k n="Orario ultima transazione"/>
     <k n="P/U"/>
     <k n="Prezzo"/>
-    <k n="Prezzo (orario esteso)"/>
     <k n="Sede centrale" t="s"/>
     <k n="Settore" t="s"/>
     <k n="Simbolo azionario" t="s"/>
@@ -920,7 +977,7 @@
 <file path=xl/richData/rdsupportingpropertybag.xml><?xml version="1.0" encoding="utf-8"?>
 <supportingPropertyBags xmlns="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2">
   <spbArrays count="2">
-    <a count="46">
+    <a count="43">
       <v t="s">%EntityServiceId</v>
       <v t="s">_Format</v>
       <v t="s">%IsRefreshable</v>
@@ -932,16 +989,13 @@
       <v t="s">Nome</v>
       <v t="s">_SubLabel</v>
       <v t="s">Prezzo</v>
-      <v t="s">Prezzo (orario esteso)</v>
       <v t="s">Exchange</v>
       <v t="s">Nome ufficiale</v>
       <v t="s">Orario ultima transazione</v>
       <v t="s">Simbolo dell'azione</v>
       <v t="s">Simbolo azionario</v>
       <v t="s">Variazione</v>
-      <v t="s">Cambia (orario prolungato)</v>
       <v t="s">Variazione (%)</v>
-      <v t="s">Cambia % (orario prolungato)</v>
       <v t="s">Valuta</v>
       <v t="s">Chiusura precedente</v>
       <v t="s">Apri</v>
@@ -1044,12 +1098,9 @@
       <v>Ticker symbol</v>
       <v>Shares outstanding</v>
       <v>52 week low</v>
-      <v>Price (Extended hours)</v>
       <v>52 week high</v>
       <v>Last trade time</v>
-      <v>Change (Extended hours)</v>
       <v>Market cap</v>
-      <v>Change % (Extended hours)</v>
     </spb>
     <spb s="1">
       <v>0</v>
@@ -1086,21 +1137,15 @@
       <v>4</v>
       <v>2</v>
       <v>2</v>
-      <v>2</v>
       <v>8</v>
-      <v>2</v>
       <v>9</v>
-      <v>5</v>
     </spb>
     <spb s="5">
-      <v xml:space="preserve">alla chiusura </v>
-      <v>Origine: Nasdaq</v>
+      <v>Tempo reale Nasdaq Ultima vendita</v>
+      <v>Origine: Nasdaq Ultima vendita</v>
       <v xml:space="preserve">dalla chiusura precedente </v>
       <v xml:space="preserve">dalla chiusura precedente </v>
-      <v>Ritardato di 15 minuti</v>
       <v>GMT</v>
-      <v xml:space="preserve">dalla chiusura </v>
-      <v xml:space="preserve">dalla chiusura </v>
     </spb>
     <spb s="6">
       <v>P/E</v>
@@ -1161,7 +1206,7 @@
       <v>8</v>
       <v>11</v>
     </spb>
-    <spb s="8">
+    <spb s="5">
       <v>Ritardato di 15 minuti</v>
       <v>Borsa Italia</v>
       <v xml:space="preserve">dalla chiusura precedente </v>
@@ -1189,7 +1234,7 @@
       <v>8</v>
       <v>11</v>
     </spb>
-    <spb s="9">
+    <spb s="8">
       <v>Ritardato di 15 minuti</v>
       <v xml:space="preserve">dalla chiusura precedente </v>
       <v xml:space="preserve">dalla chiusura precedente </v>
@@ -1200,7 +1245,7 @@
 </file>
 
 <file path=xl/richData/rdsupportingpropertybagstructure.xml><?xml version="1.0" encoding="utf-8"?>
-<spbStructures xmlns="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" count="10">
+<spbStructures xmlns="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" count="9">
   <s>
     <k n="P/U" t="s"/>
     <k n="Apri" t="s"/>
@@ -1231,12 +1276,9 @@
     <k n="Simbolo dell'azione" t="s"/>
     <k n="Azioni in circolazione" t="s"/>
     <k n="Minimo di 52 settimane" t="s"/>
-    <k n="Prezzo (orario esteso)" t="s"/>
     <k n="Massimo in 52 settimane" t="s"/>
     <k n="Orario ultima transazione" t="s"/>
-    <k n="Cambia (orario prolungato)" t="s"/>
     <k n="Capitalizzazione di mercato" t="s"/>
-    <k n="Cambia % (orario prolungato)" t="s"/>
   </s>
   <s>
     <k n="^Order" t="spba"/>
@@ -1272,22 +1314,16 @@
     <k n="Chiusura precedente" t="i"/>
     <k n="Azioni in circolazione" t="i"/>
     <k n="Minimo di 52 settimane" t="i"/>
-    <k n="Prezzo (orario esteso)" t="i"/>
     <k n="Massimo in 52 settimane" t="i"/>
     <k n="Orario ultima transazione" t="i"/>
-    <k n="Cambia (orario prolungato)" t="i"/>
     <k n="Capitalizzazione di mercato" t="i"/>
-    <k n="Cambia % (orario prolungato)" t="i"/>
   </s>
   <s>
     <k n="Prezzo" t="s"/>
     <k n="ExchangeID" t="s"/>
     <k n="Variazione" t="s"/>
     <k n="Variazione (%)" t="s"/>
-    <k n="Prezzo (orario esteso)" t="s"/>
     <k n="Orario ultima transazione" t="s"/>
-    <k n="Cambia (orario prolungato)" t="s"/>
-    <k n="Cambia % (orario prolungato)" t="s"/>
   </s>
   <s>
     <k n="P/U" t="s"/>
@@ -1342,13 +1378,6 @@
     <k n="Massimo in 52 settimane" t="i"/>
     <k n="Orario ultima transazione" t="i"/>
     <k n="Capitalizzazione di mercato" t="i"/>
-  </s>
-  <s>
-    <k n="Prezzo" t="s"/>
-    <k n="ExchangeID" t="s"/>
-    <k n="Variazione" t="s"/>
-    <k n="Variazione (%)" t="s"/>
-    <k n="Orario ultima transazione" t="s"/>
   </s>
   <s>
     <k n="Prezzo" t="s"/>
@@ -1709,34 +1738,35 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:Q5"/>
+  <dimension ref="A1:V17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
     <col min="1" max="1" width="33.734375" customWidth="1"/>
-    <col min="2" max="2" width="8.3125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.9453125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="17.83984375" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="16.26171875" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="14.15625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="8.734375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.05078125" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="14" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="12.578125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="16.3671875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="26.62890625" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="11.3671875" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="24.41796875" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="19.15625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="16.26171875" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="9.5234375" bestFit="1" customWidth="1"/>
-    <col min="15" max="16" width="4.15625" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="11.5234375" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="21.20703125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="24.41796875" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="19.15625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="16.26171875" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="9.5234375" bestFit="1" customWidth="1"/>
+    <col min="16" max="17" width="4.15625" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="11.5234375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" x14ac:dyDescent="0.55000000000000004">
-      <c r="A1" s="32" t="s">
+    <row r="1" spans="1:22" x14ac:dyDescent="0.55000000000000004">
+      <c r="A1" s="29" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
@@ -1767,298 +1797,471 @@
         <v>52</v>
       </c>
       <c r="K1" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="L1" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="M1" s="39" t="s">
         <v>51</v>
       </c>
-      <c r="M1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="N1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="O1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="P1" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="Q1" s="1" t="s">
-        <v>5</v>
-      </c>
+      <c r="N1" s="30"/>
+      <c r="O1" s="30"/>
+      <c r="P1" s="30"/>
+      <c r="Q1" s="30"/>
+      <c r="R1" s="30"/>
+      <c r="S1" s="31"/>
+      <c r="T1" s="31"/>
+      <c r="U1" s="31"/>
+      <c r="V1" s="35"/>
     </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="2" spans="1:22" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" t="e" vm="1">
         <v>#VALUE!</v>
       </c>
-      <c r="B2" s="30" cm="1">
+      <c r="B2" s="27" cm="1">
         <f t="array" aca="1" ref="B2" ca="1">_FV(A2,"Prezzo")</f>
-        <v>205.01</v>
-      </c>
-      <c r="C2" s="19" cm="1">
+        <v>206.85679999999999</v>
+      </c>
+      <c r="C2" s="18" cm="1">
         <f t="array" aca="1" ref="C2" ca="1">_FV(A2,"Capitalizzazione di mercato",TRUE)</f>
         <v>2176459000000</v>
       </c>
-      <c r="D2" s="24">
+      <c r="D2" s="23">
         <f ca="1">C2/1000000000</f>
         <v>2176.4589999999998</v>
       </c>
-      <c r="E2" s="24">
+      <c r="E2" s="23">
         <f>(AMZN!G22-AMZN!G24)</f>
         <v>67.040000000000006</v>
       </c>
-      <c r="F2" s="24">
+      <c r="F2" s="23">
         <f ca="1">D2+E2</f>
         <v>2243.4989999999998</v>
       </c>
-      <c r="G2" s="24">
+      <c r="G2" s="23">
         <f>AMZN!G2</f>
         <v>650.30999999999995</v>
       </c>
-      <c r="H2" s="24">
+      <c r="H2" s="23">
         <f>AMZN!G10</f>
         <v>130.24</v>
       </c>
-      <c r="I2" s="24">
+      <c r="I2" s="23">
         <f>AMZN!G12</f>
         <v>65.94</v>
       </c>
-      <c r="J2" s="24">
+      <c r="J2" s="23">
         <f>AMZN!G15</f>
         <v>6.14</v>
       </c>
-      <c r="K2" s="24">
+      <c r="K2" s="23">
+        <f>AMZN!G23</f>
+        <v>305.87</v>
+      </c>
+      <c r="L2" s="23">
         <f>AMZN!G27</f>
         <v>28.82</v>
       </c>
-      <c r="L2" s="24">
+      <c r="M2" s="23">
         <f>AMZN!G35</f>
         <v>42.22</v>
       </c>
-      <c r="M2" s="28">
+      <c r="N2" s="32"/>
+      <c r="O2" s="33"/>
+      <c r="P2" s="33"/>
+      <c r="Q2" s="33"/>
+      <c r="R2" s="32"/>
+      <c r="S2" s="34"/>
+      <c r="T2" s="35"/>
+      <c r="U2" s="32"/>
+      <c r="V2" s="35"/>
+    </row>
+    <row r="3" spans="1:22" x14ac:dyDescent="0.55000000000000004">
+      <c r="A3" t="e" vm="2">
+        <v>#VALUE!</v>
+      </c>
+      <c r="B3" s="28" cm="1">
+        <f t="array" aca="1" ref="B3" ca="1">_FV(A3,"Prezzo")</f>
+        <v>7.7480000000000002</v>
+      </c>
+      <c r="C3" s="19" cm="1">
+        <f t="array" aca="1" ref="C3" ca="1">_FV(A3,"Capitalizzazione di mercato",TRUE)</f>
+        <v>11105730000</v>
+      </c>
+      <c r="D3" s="23">
+        <f ca="1">C3/1000000000</f>
+        <v>11.105729999999999</v>
+      </c>
+      <c r="E3" s="23">
+        <f>BPER!G14-BPER!G16</f>
+        <v>111.56</v>
+      </c>
+      <c r="F3" s="23">
+        <f t="shared" ref="F3:F5" ca="1" si="0">D3+E3</f>
+        <v>122.66573</v>
+      </c>
+      <c r="G3" s="23">
+        <f>BPER!G2</f>
+        <v>5.86</v>
+      </c>
+      <c r="I3" s="23">
+        <f>BPER!G4</f>
+        <v>1.39</v>
+      </c>
+      <c r="J3" s="23">
+        <f>BPER!G7</f>
+        <v>1.92</v>
+      </c>
+      <c r="K3" s="23">
+        <f>BPER!G15</f>
+        <v>11.99</v>
+      </c>
+      <c r="L3" s="23">
+        <f>BPER!G18</f>
+        <v>16.64</v>
+      </c>
+      <c r="M3" s="23">
+        <f>BPER!G25</f>
+        <v>2.66</v>
+      </c>
+      <c r="N3" s="32"/>
+      <c r="O3" s="33"/>
+      <c r="P3" s="33"/>
+      <c r="Q3" s="33"/>
+      <c r="R3" s="32"/>
+      <c r="S3" s="34"/>
+      <c r="T3" s="35"/>
+      <c r="U3" s="32"/>
+      <c r="V3" s="35"/>
+    </row>
+    <row r="4" spans="1:22" x14ac:dyDescent="0.55000000000000004">
+      <c r="A4" t="e" vm="3">
+        <v>#VALUE!</v>
+      </c>
+      <c r="B4" s="28">
+        <v>44</v>
+      </c>
+      <c r="C4" s="19" cm="1">
+        <f t="array" aca="1" ref="C4" ca="1">_FV(A4,"Capitalizzazione di mercato",TRUE)</f>
+        <v>8710555000</v>
+      </c>
+      <c r="D4" s="23">
+        <f ca="1">C4/1000000000</f>
+        <v>8.7105549999999994</v>
+      </c>
+      <c r="E4" s="23">
+        <f>BUZZI!G22-BUZZI!G24</f>
+        <v>-0.43000000000000016</v>
+      </c>
+      <c r="F4" s="23">
+        <f t="shared" ca="1" si="0"/>
+        <v>8.2805549999999997</v>
+      </c>
+      <c r="G4" s="23">
+        <f>BUZZI!G2</f>
+        <v>4.3099999999999996</v>
+      </c>
+      <c r="H4" s="23">
+        <f>BUZZI!G10</f>
+        <v>1.32</v>
+      </c>
+      <c r="I4" s="23">
+        <f>BUZZI!G12</f>
+        <v>0.94</v>
+      </c>
+      <c r="J4" s="23">
+        <f>BUZZI!G15</f>
+        <v>5.0999999999999996</v>
+      </c>
+      <c r="K4" s="23">
+        <f>BUZZI!G23</f>
+        <v>5.63</v>
+      </c>
+      <c r="L4" s="23">
+        <f>BUZZI!G27</f>
+        <v>30.39</v>
+      </c>
+      <c r="M4" s="23">
+        <f>BUZZI!G35</f>
+        <v>0.55000000000000004</v>
+      </c>
+      <c r="N4" s="32"/>
+      <c r="O4" s="33"/>
+      <c r="P4" s="33"/>
+      <c r="Q4" s="33"/>
+      <c r="R4" s="32"/>
+      <c r="S4" s="34"/>
+      <c r="T4" s="35"/>
+      <c r="U4" s="32"/>
+      <c r="V4" s="35"/>
+    </row>
+    <row r="5" spans="1:22" x14ac:dyDescent="0.55000000000000004">
+      <c r="A5" t="e" vm="4">
+        <v>#VALUE!</v>
+      </c>
+      <c r="B5" s="27" cm="1">
+        <f t="array" aca="1" ref="B5" ca="1">_FV(A5,"Prezzo")</f>
+        <v>137.59299999999999</v>
+      </c>
+      <c r="C5" s="18" cm="1">
+        <f t="array" aca="1" ref="C5" ca="1">_FV(A5,"Capitalizzazione di mercato",TRUE)</f>
+        <v>3357269199999</v>
+      </c>
+      <c r="D5" s="23">
+        <f ca="1">C5/1000000000</f>
+        <v>3357.2691999990002</v>
+      </c>
+      <c r="E5" s="23">
+        <f>NVDA!G22-NVDA!G24</f>
+        <v>-4.9400000000000013</v>
+      </c>
+      <c r="F5" s="23">
+        <f t="shared" ca="1" si="0"/>
+        <v>3352.3291999990001</v>
+      </c>
+      <c r="G5" s="23">
+        <f>NVDA!G2</f>
+        <v>148.52000000000001</v>
+      </c>
+      <c r="H5" s="23">
+        <f>NVDA!G10</f>
+        <v>89.03</v>
+      </c>
+      <c r="I5" s="23">
+        <f>NVDA!G12</f>
+        <v>76.77</v>
+      </c>
+      <c r="J5" s="23">
+        <f>NVDA!G15</f>
+        <v>3.1</v>
+      </c>
+      <c r="K5" s="23">
+        <f>NVDA!G23</f>
+        <v>83.84</v>
+      </c>
+      <c r="L5" s="23">
+        <f>NVDA!G27</f>
+        <v>3.44</v>
+      </c>
+      <c r="M5" s="23">
+        <f>NVDA!G35</f>
+        <v>73.63</v>
+      </c>
+      <c r="N5" s="32"/>
+      <c r="O5" s="33"/>
+      <c r="P5" s="33"/>
+      <c r="Q5" s="33"/>
+      <c r="R5" s="32"/>
+      <c r="S5" s="34"/>
+      <c r="T5" s="35"/>
+      <c r="U5" s="32"/>
+      <c r="V5" s="35"/>
+    </row>
+    <row r="9" spans="1:22" x14ac:dyDescent="0.55000000000000004">
+      <c r="A9" s="36"/>
+      <c r="B9" s="36" t="s">
+        <v>1</v>
+      </c>
+      <c r="C9" s="36" t="s">
+        <v>2</v>
+      </c>
+      <c r="D9" s="36" t="s">
+        <v>3</v>
+      </c>
+      <c r="E9" s="36" t="s">
+        <v>4</v>
+      </c>
+      <c r="F9" s="36" t="s">
+        <v>5</v>
+      </c>
+      <c r="G9" s="37" t="s">
+        <v>55</v>
+      </c>
+      <c r="H9" s="37" t="s">
+        <v>56</v>
+      </c>
+      <c r="I9" s="37" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="10" spans="1:22" x14ac:dyDescent="0.55000000000000004">
+      <c r="A10" s="38" t="s">
+        <v>62</v>
+      </c>
+      <c r="B10" s="32">
         <f>H2/G2</f>
         <v>0.20027371561255405</v>
       </c>
-      <c r="N2" s="29">
+      <c r="C10" s="33">
         <f ca="1">F2/H2</f>
         <v>17.225882985257982</v>
       </c>
-      <c r="O2" s="29">
-        <f ca="1">D2/I2</f>
-        <v>33.00665756748559</v>
-      </c>
-      <c r="P2" s="29">
-        <f ca="1">B2/K2</f>
-        <v>7.113462873004857</v>
-      </c>
-      <c r="Q2" s="28">
-        <f ca="1">L2/D2</f>
+      <c r="D10" s="33">
+        <f ca="1">B2/J2</f>
+        <v>33.690032573289905</v>
+      </c>
+      <c r="E10" s="33">
+        <f ca="1">D2/K2</f>
+        <v>7.1156340929152906</v>
+      </c>
+      <c r="F10" s="32">
+        <f ca="1">M2/D2</f>
         <v>1.9398481662186148E-2</v>
       </c>
+      <c r="G10" s="34">
+        <f>I2/K2</f>
+        <v>0.21558178311047177</v>
+      </c>
+      <c r="H10" s="35"/>
+      <c r="I10" s="32">
+        <f>AMZN!G34/AMZN!G10</f>
+        <v>0.71475737100737102</v>
+      </c>
     </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.55000000000000004">
-      <c r="A3" t="e" vm="2">
-        <v>#VALUE!</v>
-      </c>
-      <c r="B3" s="31" cm="1">
-        <f t="array" aca="1" ref="B3" ca="1">_FV(A3,"Prezzo")</f>
-        <v>7.8120000000000003</v>
-      </c>
-      <c r="C3" s="20" cm="1">
-        <f t="array" aca="1" ref="C3" ca="1">_FV(A3,"Capitalizzazione di mercato",TRUE)</f>
-        <v>11105730000</v>
-      </c>
-      <c r="D3" s="24">
-        <f ca="1">C3/1000000000</f>
-        <v>11.105729999999999</v>
-      </c>
-      <c r="E3" s="24">
-        <f>BPER!G14-BPER!G16</f>
-        <v>111.56</v>
-      </c>
-      <c r="F3" s="24">
-        <f t="shared" ref="F3:F5" ca="1" si="0">D3+E3</f>
-        <v>122.66573</v>
-      </c>
-      <c r="G3" s="24">
-        <f>BPER!G2</f>
-        <v>5.86</v>
-      </c>
-      <c r="I3" s="24">
-        <f>BPER!G4</f>
-        <v>1.39</v>
-      </c>
-      <c r="J3" s="24">
-        <f>BPER!G7</f>
-        <v>1.92</v>
-      </c>
-      <c r="K3" s="24">
-        <f>BPER!G18</f>
-        <v>16.64</v>
-      </c>
-      <c r="L3" s="24">
-        <f>BPER!G25</f>
-        <v>2.66</v>
-      </c>
-      <c r="M3" s="28">
-        <f t="shared" ref="M3:M5" si="1">H3/G3</f>
+    <row r="11" spans="1:22" x14ac:dyDescent="0.55000000000000004">
+      <c r="A11" s="38" t="s">
+        <v>59</v>
+      </c>
+      <c r="B11" s="32">
+        <f t="shared" ref="B11:B13" si="1">H3/G3</f>
         <v>0</v>
       </c>
-      <c r="N3" s="29" t="e">
-        <f t="shared" ref="N3:N5" ca="1" si="2">F3/H3</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="O3" s="29">
-        <f t="shared" ref="O3:O5" ca="1" si="3">D3/I3</f>
-        <v>7.9897338129496402</v>
-      </c>
-      <c r="P3" s="29">
-        <f t="shared" ref="P3:P5" ca="1" si="4">B3/K3</f>
-        <v>0.46947115384615384</v>
-      </c>
-      <c r="Q3" s="28">
-        <f t="shared" ref="Q3:Q5" ca="1" si="5">L3/D3</f>
+      <c r="C11" s="33">
+        <v>0</v>
+      </c>
+      <c r="D11" s="33">
+        <f t="shared" ref="D11:D13" ca="1" si="2">B3/J3</f>
+        <v>4.0354166666666673</v>
+      </c>
+      <c r="E11" s="33">
+        <f t="shared" ref="E11:E13" ca="1" si="3">D3/K3</f>
+        <v>0.92624937447873223</v>
+      </c>
+      <c r="F11" s="32">
+        <f t="shared" ref="F11:F13" ca="1" si="4">M3/D3</f>
         <v>0.23951599759763656</v>
       </c>
+      <c r="G11" s="34">
+        <f t="shared" ref="G11:G13" si="5">I3/K3</f>
+        <v>0.11592994161801501</v>
+      </c>
+      <c r="H11" s="35"/>
+      <c r="I11" s="32">
+        <v>0</v>
+      </c>
     </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.55000000000000004">
-      <c r="A4" t="e" vm="3">
-        <v>#VALUE!</v>
-      </c>
-      <c r="B4" s="31" cm="1">
-        <f t="array" aca="1" ref="B4" ca="1">_FV(A4,"Prezzo")</f>
-        <v>25.85</v>
-      </c>
-      <c r="C4" s="20" cm="1">
-        <f t="array" aca="1" ref="C4" ca="1">_FV(A4,"Capitalizzazione di mercato",TRUE)</f>
-        <v>8710555000</v>
-      </c>
-      <c r="D4" s="24">
-        <f ca="1">C4/1000000000</f>
-        <v>8.7105549999999994</v>
-      </c>
-      <c r="E4" s="24">
-        <f>BUZZI!G22-BUZZI!G24</f>
-        <v>-0.43000000000000016</v>
-      </c>
-      <c r="F4" s="24">
-        <f t="shared" ca="1" si="0"/>
-        <v>8.2805549999999997</v>
-      </c>
-      <c r="G4" s="24">
-        <f>BUZZI!G2</f>
-        <v>4.3099999999999996</v>
-      </c>
-      <c r="H4" s="24">
-        <f>BUZZI!G10</f>
-        <v>1.32</v>
-      </c>
-      <c r="I4" s="24">
-        <f>BUZZI!G12</f>
-        <v>0.94</v>
-      </c>
-      <c r="J4" s="24">
-        <f>BUZZI!G15</f>
-        <v>5.0999999999999996</v>
-      </c>
-      <c r="K4" s="24">
-        <f>BUZZI!G27</f>
-        <v>30.39</v>
-      </c>
-      <c r="L4" s="24">
-        <f>BUZZI!G35</f>
-        <v>0.55000000000000004</v>
-      </c>
-      <c r="M4" s="28">
+    <row r="12" spans="1:22" x14ac:dyDescent="0.55000000000000004">
+      <c r="A12" s="38" t="s">
+        <v>60</v>
+      </c>
+      <c r="B12" s="32">
         <f t="shared" si="1"/>
         <v>0.30626450116009285</v>
       </c>
-      <c r="N4" s="29">
-        <f t="shared" ca="1" si="2"/>
+      <c r="C12" s="33">
+        <f t="shared" ref="C11:C13" ca="1" si="6">F4/H4</f>
         <v>6.2731477272727263</v>
       </c>
-      <c r="O4" s="29">
+      <c r="D12" s="33">
+        <f t="shared" si="2"/>
+        <v>8.6274509803921582</v>
+      </c>
+      <c r="E12" s="33">
         <f t="shared" ca="1" si="3"/>
-        <v>9.2665478723404249</v>
-      </c>
-      <c r="P4" s="29">
+        <v>1.5471678507992894</v>
+      </c>
+      <c r="F12" s="32">
         <f t="shared" ca="1" si="4"/>
-        <v>0.85060875287923665</v>
-      </c>
-      <c r="Q4" s="28">
-        <f t="shared" ca="1" si="5"/>
         <v>6.3141786028559618E-2</v>
       </c>
+      <c r="G12" s="34">
+        <f t="shared" si="5"/>
+        <v>0.1669626998223801</v>
+      </c>
+      <c r="H12" s="35"/>
+      <c r="I12" s="32">
+        <f>BUZZI!G34/BUZZI!G10</f>
+        <v>0.34090909090909088</v>
+      </c>
     </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.55000000000000004">
-      <c r="A5" t="e" vm="4">
-        <v>#VALUE!</v>
-      </c>
-      <c r="B5" s="30" cm="1">
-        <f t="array" aca="1" ref="B5" ca="1">_FV(A5,"Prezzo")</f>
-        <v>135.13</v>
-      </c>
-      <c r="C5" s="19" cm="1">
-        <f t="array" aca="1" ref="C5" ca="1">_FV(A5,"Capitalizzazione di mercato",TRUE)</f>
-        <v>3297172000000</v>
-      </c>
-      <c r="D5" s="24">
-        <f ca="1">C5/1000000000</f>
-        <v>3297.172</v>
-      </c>
-      <c r="E5" s="24">
-        <f>NVDA!G22-NVDA!G24</f>
-        <v>-4.9400000000000013</v>
-      </c>
-      <c r="F5" s="24">
-        <f t="shared" ca="1" si="0"/>
-        <v>3292.232</v>
-      </c>
-      <c r="G5" s="24">
-        <f>NVDA!G2</f>
-        <v>148.52000000000001</v>
-      </c>
-      <c r="H5" s="24">
-        <f>NVDA!G10</f>
-        <v>89.03</v>
-      </c>
-      <c r="I5" s="24">
-        <f>NVDA!G12</f>
-        <v>76.77</v>
-      </c>
-      <c r="J5" s="24">
-        <f>NVDA!G15</f>
-        <v>3.1</v>
-      </c>
-      <c r="K5" s="24">
-        <f>NVDA!G27</f>
-        <v>3.44</v>
-      </c>
-      <c r="L5" s="24">
-        <f>NVDA!G35</f>
-        <v>73.63</v>
-      </c>
-      <c r="M5" s="28">
+    <row r="13" spans="1:22" x14ac:dyDescent="0.55000000000000004">
+      <c r="A13" s="38" t="s">
+        <v>61</v>
+      </c>
+      <c r="B13" s="32">
         <f t="shared" si="1"/>
         <v>0.59944788580662534</v>
       </c>
-      <c r="N5" s="29">
+      <c r="C13" s="33">
+        <f t="shared" ca="1" si="6"/>
+        <v>37.653927889464228</v>
+      </c>
+      <c r="D13" s="33">
         <f t="shared" ca="1" si="2"/>
-        <v>36.978905986746042</v>
-      </c>
-      <c r="O5" s="29">
+        <v>44.384838709677418</v>
+      </c>
+      <c r="E13" s="33">
         <f t="shared" ca="1" si="3"/>
-        <v>42.948703920802402</v>
-      </c>
-      <c r="P5" s="29">
+        <v>40.043764312965173</v>
+      </c>
+      <c r="F13" s="32">
         <f t="shared" ca="1" si="4"/>
-        <v>39.281976744186046</v>
-      </c>
-      <c r="Q5" s="28">
-        <f t="shared" ca="1" si="5"/>
-        <v>2.233125842388568E-2</v>
-      </c>
+        <v>2.1931515053967648E-2</v>
+      </c>
+      <c r="G13" s="34">
+        <f t="shared" si="5"/>
+        <v>0.91567270992366401</v>
+      </c>
+      <c r="H13" s="35"/>
+      <c r="I13" s="32">
+        <f>NVDA!G34/NVDA!G10</f>
+        <v>4.5939570931146805E-2</v>
+      </c>
+    </row>
+    <row r="14" spans="1:22" x14ac:dyDescent="0.55000000000000004">
+      <c r="A14" s="31"/>
+      <c r="B14" s="35"/>
+      <c r="C14" s="35"/>
+      <c r="D14" s="35"/>
+      <c r="E14" s="35"/>
+      <c r="F14" s="35"/>
+      <c r="G14" s="35"/>
+      <c r="H14" s="35"/>
+      <c r="I14" s="35"/>
+    </row>
+    <row r="15" spans="1:22" x14ac:dyDescent="0.55000000000000004">
+      <c r="A15" s="31"/>
+      <c r="B15" s="35"/>
+      <c r="C15" s="35"/>
+      <c r="D15" s="35"/>
+      <c r="E15" s="35"/>
+      <c r="F15" s="35"/>
+      <c r="G15" s="35"/>
+      <c r="H15" s="35"/>
+      <c r="I15" s="35"/>
+    </row>
+    <row r="16" spans="1:22" x14ac:dyDescent="0.55000000000000004">
+      <c r="A16" s="31"/>
+      <c r="B16" s="32"/>
+      <c r="C16" s="32"/>
+      <c r="D16" s="32"/>
+      <c r="E16" s="32"/>
+      <c r="F16" s="35"/>
+      <c r="G16" s="35"/>
+      <c r="H16" s="35"/>
+      <c r="I16" s="35"/>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+      <c r="A17" s="35"/>
+      <c r="B17" s="35"/>
+      <c r="C17" s="35"/>
+      <c r="D17" s="35"/>
+      <c r="E17" s="35"/>
+      <c r="F17" s="35"/>
+      <c r="G17" s="35"/>
+      <c r="H17" s="35"/>
+      <c r="I17" s="35"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2069,8 +2272,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:XFB36"/>
   <sheetViews>
-    <sheetView topLeftCell="A5" workbookViewId="0">
-      <selection activeCell="G27" sqref="G27"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I7" sqref="I7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -2110,22 +2313,22 @@
       <c r="A2" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="B2" s="21">
+      <c r="B2" s="20">
         <v>386.06</v>
       </c>
-      <c r="C2" s="21">
+      <c r="C2" s="20">
         <v>469.82</v>
       </c>
-      <c r="D2" s="21">
+      <c r="D2" s="20">
         <v>513.98</v>
       </c>
-      <c r="E2" s="21">
+      <c r="E2" s="20">
         <v>574.79</v>
       </c>
-      <c r="F2" s="21">
+      <c r="F2" s="20">
         <v>637.96</v>
       </c>
-      <c r="G2" s="21">
+      <c r="G2" s="20">
         <v>650.30999999999995</v>
       </c>
     </row>
@@ -2133,22 +2336,22 @@
       <c r="A3" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="B3" s="26">
+      <c r="B3" s="25">
         <v>0.37619999999999998</v>
       </c>
-      <c r="C3" s="26">
+      <c r="C3" s="25">
         <v>0.217</v>
       </c>
-      <c r="D3" s="26">
+      <c r="D3" s="25">
         <v>9.4E-2</v>
       </c>
-      <c r="E3" s="26">
+      <c r="E3" s="25">
         <v>0.1183</v>
       </c>
-      <c r="F3" s="26">
+      <c r="F3" s="25">
         <v>0.1099</v>
       </c>
-      <c r="G3" s="26">
+      <c r="G3" s="25">
         <v>0.1008</v>
       </c>
     </row>
@@ -2156,22 +2359,22 @@
       <c r="A4" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="B4" s="21">
+      <c r="B4" s="20">
         <v>152.76</v>
       </c>
-      <c r="C4" s="21">
+      <c r="C4" s="20">
         <v>197.48</v>
       </c>
-      <c r="D4" s="21">
+      <c r="D4" s="20">
         <v>225.15</v>
       </c>
-      <c r="E4" s="21">
+      <c r="E4" s="20">
         <v>270.05</v>
       </c>
-      <c r="F4" s="21">
+      <c r="F4" s="20">
         <v>311.67</v>
       </c>
-      <c r="G4" s="21">
+      <c r="G4" s="20">
         <v>319.68</v>
       </c>
     </row>
@@ -2179,22 +2382,22 @@
       <c r="A5" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="B5" s="26">
+      <c r="B5" s="25">
         <v>0.3957</v>
       </c>
-      <c r="C5" s="26">
+      <c r="C5" s="25">
         <v>0.42030000000000001</v>
       </c>
-      <c r="D5" s="26">
+      <c r="D5" s="25">
         <v>0.43809999999999999</v>
       </c>
-      <c r="E5" s="26">
+      <c r="E5" s="25">
         <v>0.4698</v>
       </c>
-      <c r="F5" s="26">
+      <c r="F5" s="25">
         <v>0.48849999999999999</v>
       </c>
-      <c r="G5" s="26">
+      <c r="G5" s="25">
         <v>0.49159999999999998</v>
       </c>
       <c r="H5"/>
@@ -4543,22 +4746,22 @@
       <c r="A6" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="B6" s="21">
+      <c r="B6" s="20">
         <v>22.9</v>
       </c>
-      <c r="C6" s="21">
+      <c r="C6" s="20">
         <v>24.88</v>
       </c>
-      <c r="D6" s="21">
+      <c r="D6" s="20">
         <v>12.25</v>
       </c>
-      <c r="E6" s="21">
+      <c r="E6" s="20">
         <v>36.85</v>
       </c>
-      <c r="F6" s="21">
+      <c r="F6" s="20">
         <v>68.59</v>
       </c>
-      <c r="G6" s="21">
+      <c r="G6" s="20">
         <v>71.69</v>
       </c>
     </row>
@@ -4566,22 +4769,22 @@
       <c r="A7" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="B7" s="26">
+      <c r="B7" s="25">
         <v>5.9299999999999999E-2</v>
       </c>
-      <c r="C7" s="26">
+      <c r="C7" s="25">
         <v>5.2999999999999999E-2</v>
       </c>
-      <c r="D7" s="26">
+      <c r="D7" s="25">
         <v>2.3800000000000002E-2</v>
       </c>
-      <c r="E7" s="26">
+      <c r="E7" s="25">
         <v>6.4100000000000004E-2</v>
       </c>
-      <c r="F7" s="26">
+      <c r="F7" s="25">
         <v>0.1075</v>
       </c>
-      <c r="G7" s="26">
+      <c r="G7" s="25">
         <v>0.11020000000000001</v>
       </c>
       <c r="H7"/>
@@ -6930,22 +7133,22 @@
       <c r="A8" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="B8" s="21">
+      <c r="B8" s="20">
         <v>25.27</v>
       </c>
-      <c r="C8" s="21">
+      <c r="C8" s="20">
         <v>39.51</v>
       </c>
-      <c r="D8" s="21">
+      <c r="D8" s="20">
         <v>-4.5599999999999996</v>
       </c>
-      <c r="E8" s="21">
+      <c r="E8" s="20">
         <v>37.79</v>
       </c>
-      <c r="F8" s="21">
+      <c r="F8" s="20">
         <v>66.34</v>
       </c>
-      <c r="G8" s="21">
+      <c r="G8" s="20">
         <v>74.86</v>
       </c>
     </row>
@@ -6953,22 +7156,22 @@
       <c r="A9" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="B9" s="26">
+      <c r="B9" s="25">
         <v>6.5500000000000003E-2</v>
       </c>
-      <c r="C9" s="26">
+      <c r="C9" s="25">
         <v>8.4099999999999994E-2</v>
       </c>
-      <c r="D9" s="26">
+      <c r="D9" s="25">
         <v>-8.8999999999999999E-3</v>
       </c>
-      <c r="E9" s="26">
+      <c r="E9" s="25">
         <v>6.5699999999999995E-2</v>
       </c>
-      <c r="F9" s="26">
+      <c r="F9" s="25">
         <v>0.104</v>
       </c>
-      <c r="G9" s="26">
+      <c r="G9" s="25">
         <v>0.11509999999999999</v>
       </c>
       <c r="H9"/>
@@ -9317,22 +9520,22 @@
       <c r="A10" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="B10" s="21">
+      <c r="B10" s="20">
         <v>50.52</v>
       </c>
-      <c r="C10" s="21">
+      <c r="C10" s="20">
         <v>73.81</v>
       </c>
-      <c r="D10" s="21">
+      <c r="D10" s="20">
         <v>37.36</v>
       </c>
-      <c r="E10" s="21">
+      <c r="E10" s="20">
         <v>86.45</v>
       </c>
-      <c r="F10" s="21">
+      <c r="F10" s="20">
         <v>119.14</v>
       </c>
-      <c r="G10" s="21">
+      <c r="G10" s="20">
         <v>130.24</v>
       </c>
     </row>
@@ -9340,22 +9543,22 @@
       <c r="A11" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="B11" s="26">
+      <c r="B11" s="25">
         <v>0.13089999999999999</v>
       </c>
-      <c r="C11" s="26">
+      <c r="C11" s="25">
         <v>0.15709999999999999</v>
       </c>
-      <c r="D11" s="26">
+      <c r="D11" s="25">
         <v>7.2700000000000001E-2</v>
       </c>
-      <c r="E11" s="26">
+      <c r="E11" s="25">
         <v>0.15040000000000001</v>
       </c>
-      <c r="F11" s="26">
+      <c r="F11" s="25">
         <v>0.1867</v>
       </c>
-      <c r="G11" s="26">
+      <c r="G11" s="25">
         <v>0.20030000000000001</v>
       </c>
       <c r="H11"/>
@@ -11704,22 +11907,22 @@
       <c r="A12" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="B12" s="21">
+      <c r="B12" s="20">
         <v>21.33</v>
       </c>
-      <c r="C12" s="21">
+      <c r="C12" s="20">
         <v>33.36</v>
       </c>
-      <c r="D12" s="21">
+      <c r="D12" s="20">
         <v>-2.72</v>
       </c>
-      <c r="E12" s="21">
+      <c r="E12" s="20">
         <v>30.43</v>
       </c>
-      <c r="F12" s="21">
+      <c r="F12" s="20">
         <v>59.25</v>
       </c>
-      <c r="G12" s="21">
+      <c r="G12" s="20">
         <v>65.94</v>
       </c>
     </row>
@@ -11727,22 +11930,22 @@
       <c r="A13" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="B13" s="26">
+      <c r="B13" s="25">
         <v>5.5300000000000002E-2</v>
       </c>
-      <c r="C13" s="26">
+      <c r="C13" s="25">
         <v>7.0999999999999994E-2</v>
       </c>
-      <c r="D13" s="26">
+      <c r="D13" s="25">
         <v>-5.3E-3</v>
       </c>
-      <c r="E13" s="26">
+      <c r="E13" s="25">
         <v>5.2900000000000003E-2</v>
       </c>
-      <c r="F13" s="26">
+      <c r="F13" s="25">
         <v>9.2899999999999996E-2</v>
       </c>
-      <c r="G13" s="26">
+      <c r="G13" s="25">
         <v>0.1014</v>
       </c>
       <c r="H13"/>
@@ -14091,22 +14294,22 @@
       <c r="A14" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="B14" s="21">
+      <c r="B14" s="20">
         <v>2.13</v>
       </c>
-      <c r="C14" s="21">
+      <c r="C14" s="20">
         <v>3.3</v>
       </c>
-      <c r="D14" s="21">
+      <c r="D14" s="20">
         <v>-0.27</v>
       </c>
-      <c r="E14" s="21">
+      <c r="E14" s="20">
         <v>2.95</v>
       </c>
-      <c r="F14" s="21">
+      <c r="F14" s="20">
         <v>5.66</v>
       </c>
-      <c r="G14" s="21">
+      <c r="G14" s="20">
         <v>6.27</v>
       </c>
     </row>
@@ -14114,22 +14317,22 @@
       <c r="A15" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="B15" s="21">
+      <c r="B15" s="20">
         <v>2.09</v>
       </c>
-      <c r="C15" s="21">
+      <c r="C15" s="20">
         <v>3.24</v>
       </c>
-      <c r="D15" s="21">
+      <c r="D15" s="20">
         <v>-0.27</v>
       </c>
-      <c r="E15" s="21">
+      <c r="E15" s="20">
         <v>2.9</v>
       </c>
-      <c r="F15" s="21">
+      <c r="F15" s="20">
         <v>5.53</v>
       </c>
-      <c r="G15" s="21">
+      <c r="G15" s="20">
         <v>6.14</v>
       </c>
     </row>
@@ -14137,22 +14340,22 @@
       <c r="A16" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="B16" s="21">
+      <c r="B16" s="20">
         <v>2.09</v>
       </c>
-      <c r="C16" s="21">
+      <c r="C16" s="20">
         <v>2.09</v>
       </c>
-      <c r="D16" s="21">
+      <c r="D16" s="20">
         <v>0.95</v>
       </c>
-      <c r="E16" s="21">
+      <c r="E16" s="20">
         <v>2.84</v>
       </c>
-      <c r="F16" s="21">
+      <c r="F16" s="20">
         <v>5.71</v>
       </c>
-      <c r="G16" s="25">
+      <c r="G16" s="24">
         <v>6.17</v>
       </c>
     </row>
@@ -14215,22 +14418,22 @@
       <c r="A20" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="B20" s="21">
+      <c r="B20" s="20">
         <v>321.2</v>
       </c>
-      <c r="C20" s="21">
+      <c r="C20" s="20">
         <v>420.55</v>
       </c>
-      <c r="D20" s="21">
+      <c r="D20" s="20">
         <v>462.68</v>
       </c>
-      <c r="E20" s="21">
+      <c r="E20" s="20">
         <v>527.85</v>
       </c>
-      <c r="F20" s="21">
+      <c r="F20" s="20">
         <v>624.89</v>
       </c>
-      <c r="G20" s="21">
+      <c r="G20" s="20">
         <v>643.26</v>
       </c>
     </row>
@@ -14238,22 +14441,22 @@
       <c r="A21" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="B21" s="21">
+      <c r="B21" s="20">
         <v>227.79</v>
       </c>
-      <c r="C21" s="21">
+      <c r="C21" s="20">
         <v>282.3</v>
       </c>
-      <c r="D21" s="21">
+      <c r="D21" s="20">
         <v>316.63</v>
       </c>
-      <c r="E21" s="21">
+      <c r="E21" s="20">
         <v>325.98</v>
       </c>
-      <c r="F21" s="21">
+      <c r="F21" s="20">
         <v>338.92</v>
       </c>
-      <c r="G21" s="21">
+      <c r="G21" s="20">
         <v>337.39</v>
       </c>
     </row>
@@ -14261,22 +14464,22 @@
       <c r="A22" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="B22" s="21">
+      <c r="B22" s="20">
         <v>84.39</v>
       </c>
-      <c r="C22" s="21">
+      <c r="C22" s="20">
         <v>116.4</v>
       </c>
-      <c r="D22" s="21">
+      <c r="D22" s="20">
         <v>140.12</v>
       </c>
-      <c r="E22" s="21">
+      <c r="E22" s="20">
         <v>135.61000000000001</v>
       </c>
-      <c r="F22" s="21">
+      <c r="F22" s="20">
         <v>130.9</v>
       </c>
-      <c r="G22" s="21">
+      <c r="G22" s="20">
         <v>133.25</v>
       </c>
     </row>
@@ -14284,22 +14487,22 @@
       <c r="A23" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="B23" s="21">
+      <c r="B23" s="20">
         <v>93.4</v>
       </c>
-      <c r="C23" s="21">
+      <c r="C23" s="20">
         <v>138.25</v>
       </c>
-      <c r="D23" s="21">
+      <c r="D23" s="20">
         <v>146.04</v>
       </c>
-      <c r="E23" s="21">
+      <c r="E23" s="20">
         <v>201.88</v>
       </c>
-      <c r="F23" s="21">
+      <c r="F23" s="20">
         <v>285.97000000000003</v>
       </c>
-      <c r="G23" s="21">
+      <c r="G23" s="20">
         <v>305.87</v>
       </c>
     </row>
@@ -14307,22 +14510,22 @@
       <c r="A24" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="B24" s="21">
+      <c r="B24" s="20">
         <v>42.12</v>
       </c>
-      <c r="C24" s="21">
+      <c r="C24" s="20">
         <v>36.22</v>
       </c>
-      <c r="D24" s="21">
+      <c r="D24" s="20">
         <v>53.89</v>
       </c>
-      <c r="E24" s="21">
+      <c r="E24" s="20">
         <v>73.39</v>
       </c>
-      <c r="F24" s="21">
+      <c r="F24" s="20">
         <v>78.78</v>
       </c>
-      <c r="G24" s="21">
+      <c r="G24" s="20">
         <v>66.209999999999994</v>
       </c>
     </row>
@@ -14330,22 +14533,22 @@
       <c r="A25" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="B25" s="21">
+      <c r="B25" s="20">
         <v>6.35</v>
       </c>
-      <c r="C25" s="21">
+      <c r="C25" s="20">
         <v>19.309999999999999</v>
       </c>
-      <c r="D25" s="21">
+      <c r="D25" s="20">
         <v>-8.6</v>
       </c>
-      <c r="E25" s="21">
+      <c r="E25" s="20">
         <v>7.43</v>
       </c>
-      <c r="F25" s="21">
+      <c r="F25" s="20">
         <v>11.44</v>
       </c>
-      <c r="G25" s="21">
+      <c r="G25" s="20">
         <v>8.4700000000000006</v>
       </c>
     </row>
@@ -14353,22 +14556,22 @@
       <c r="A26" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="B26" s="21">
+      <c r="B26" s="20">
         <v>10.039999999999999</v>
       </c>
-      <c r="C26" s="21">
+      <c r="C26" s="20">
         <v>10.14</v>
       </c>
-      <c r="D26" s="21">
+      <c r="D26" s="20">
         <v>10.199999999999999</v>
       </c>
-      <c r="E26" s="21">
+      <c r="E26" s="20">
         <v>10.33</v>
       </c>
-      <c r="F26" s="21">
+      <c r="F26" s="20">
         <v>10.52</v>
       </c>
-      <c r="G26" s="21">
+      <c r="G26" s="20">
         <v>10.52</v>
       </c>
     </row>
@@ -14376,22 +14579,22 @@
       <c r="A27" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="B27" s="21">
+      <c r="B27" s="20">
         <v>9.2799999999999994</v>
       </c>
-      <c r="C27" s="21">
+      <c r="C27" s="20">
         <v>13.58</v>
       </c>
-      <c r="D27" s="21">
+      <c r="D27" s="20">
         <v>14.26</v>
       </c>
-      <c r="E27" s="21">
+      <c r="E27" s="20">
         <v>19.440000000000001</v>
       </c>
-      <c r="F27" s="21">
+      <c r="F27" s="20">
         <v>27</v>
       </c>
-      <c r="G27" s="21">
+      <c r="G27" s="20">
         <v>28.82</v>
       </c>
     </row>
@@ -14399,22 +14602,22 @@
       <c r="A28" s="5" t="s">
         <v>34</v>
       </c>
-      <c r="B28" s="21">
+      <c r="B28" s="20">
         <v>0.9</v>
       </c>
-      <c r="C28" s="21">
+      <c r="C28" s="20">
         <v>0.84</v>
       </c>
-      <c r="D28" s="21">
+      <c r="D28" s="20">
         <v>0.96</v>
       </c>
-      <c r="E28" s="21">
+      <c r="E28" s="20">
         <v>0.67</v>
       </c>
-      <c r="F28" s="21">
+      <c r="F28" s="20">
         <v>0.46</v>
       </c>
-      <c r="G28" s="21">
+      <c r="G28" s="20">
         <v>0.44</v>
       </c>
     </row>
@@ -14454,22 +14657,22 @@
       <c r="A31" s="5" t="s">
         <v>36</v>
       </c>
-      <c r="B31" s="21">
+      <c r="B31" s="20">
         <v>66.06</v>
       </c>
-      <c r="C31" s="21">
+      <c r="C31" s="20">
         <v>46.33</v>
       </c>
-      <c r="D31" s="21">
+      <c r="D31" s="20">
         <v>46.75</v>
       </c>
-      <c r="E31" s="21">
+      <c r="E31" s="20">
         <v>84.95</v>
       </c>
-      <c r="F31" s="21">
+      <c r="F31" s="20">
         <v>115.88</v>
       </c>
-      <c r="G31" s="21">
+      <c r="G31" s="20">
         <v>113.9</v>
       </c>
     </row>
@@ -14477,22 +14680,22 @@
       <c r="A32" s="5" t="s">
         <v>37</v>
       </c>
-      <c r="B32" s="21">
+      <c r="B32" s="20">
         <v>-59.61</v>
       </c>
-      <c r="C32" s="21">
+      <c r="C32" s="20">
         <v>-58.15</v>
       </c>
-      <c r="D32" s="21">
+      <c r="D32" s="20">
         <v>-37.6</v>
       </c>
-      <c r="E32" s="21">
+      <c r="E32" s="20">
         <v>-49.83</v>
       </c>
-      <c r="F32" s="21">
+      <c r="F32" s="20">
         <v>-94.34</v>
       </c>
-      <c r="G32" s="21">
+      <c r="G32" s="20">
         <v>-106.28</v>
       </c>
     </row>
@@ -14500,22 +14703,22 @@
       <c r="A33" s="5" t="s">
         <v>38</v>
       </c>
-      <c r="B33" s="21">
+      <c r="B33" s="20">
         <v>-1.1000000000000001</v>
       </c>
-      <c r="C33" s="21">
+      <c r="C33" s="20">
         <v>6.29</v>
       </c>
-      <c r="D33" s="21">
+      <c r="D33" s="20">
         <v>9.7200000000000006</v>
       </c>
-      <c r="E33" s="21">
+      <c r="E33" s="20">
         <v>-15.88</v>
       </c>
-      <c r="F33" s="21">
+      <c r="F33" s="20">
         <v>-11.81</v>
       </c>
-      <c r="G33" s="21">
+      <c r="G33" s="20">
         <v>-10.6</v>
       </c>
     </row>
@@ -14523,22 +14726,22 @@
       <c r="A34" s="5" t="s">
         <v>39</v>
       </c>
-      <c r="B34" s="21">
+      <c r="B34" s="20">
         <v>40.14</v>
       </c>
-      <c r="C34" s="21">
+      <c r="C34" s="20">
         <v>61.05</v>
       </c>
-      <c r="D34" s="21">
+      <c r="D34" s="20">
         <v>63.65</v>
       </c>
-      <c r="E34" s="21">
+      <c r="E34" s="20">
         <v>52.73</v>
       </c>
-      <c r="F34" s="21">
+      <c r="F34" s="20">
         <v>83</v>
       </c>
-      <c r="G34" s="21">
+      <c r="G34" s="20">
         <v>93.09</v>
       </c>
     </row>
@@ -14546,22 +14749,22 @@
       <c r="A35" s="5" t="s">
         <v>40</v>
       </c>
-      <c r="B35" s="21">
+      <c r="B35" s="20">
         <v>12.44</v>
       </c>
-      <c r="C35" s="21">
+      <c r="C35" s="20">
         <v>4.8899999999999997</v>
       </c>
-      <c r="D35" s="21">
+      <c r="D35" s="20">
         <v>3.99</v>
       </c>
-      <c r="E35" s="21">
+      <c r="E35" s="20">
         <v>43.76</v>
       </c>
-      <c r="F35" s="21">
+      <c r="F35" s="20">
         <v>48.42</v>
       </c>
-      <c r="G35" s="21">
+      <c r="G35" s="20">
         <v>42.22</v>
       </c>
     </row>
@@ -14569,22 +14772,22 @@
       <c r="A36" s="5" t="s">
         <v>41</v>
       </c>
-      <c r="B36" s="21">
+      <c r="B36" s="20">
         <v>5.35</v>
       </c>
-      <c r="C36" s="21">
+      <c r="C36" s="20">
         <v>-5.54</v>
       </c>
-      <c r="D36" s="21">
+      <c r="D36" s="20">
         <v>18.87</v>
       </c>
-      <c r="E36" s="21">
+      <c r="E36" s="20">
         <v>19.23</v>
       </c>
-      <c r="F36" s="21">
+      <c r="F36" s="20">
         <v>9.7200000000000006</v>
       </c>
-      <c r="G36" s="21">
+      <c r="G36" s="20">
         <v>-2.98</v>
       </c>
     </row>
@@ -14637,22 +14840,22 @@
       <c r="A2" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="B2" s="21">
+      <c r="B2" s="20">
         <v>2.74</v>
       </c>
-      <c r="C2" s="21">
+      <c r="C2" s="20">
         <v>3.68</v>
       </c>
-      <c r="D2" s="21">
+      <c r="D2" s="20">
         <v>4.3099999999999996</v>
       </c>
-      <c r="E2" s="21">
+      <c r="E2" s="20">
         <v>5.9</v>
       </c>
-      <c r="F2" s="21">
+      <c r="F2" s="20">
         <v>5.99</v>
       </c>
-      <c r="G2" s="21">
+      <c r="G2" s="20">
         <v>5.86</v>
       </c>
     </row>
@@ -14660,22 +14863,22 @@
       <c r="A3" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="B3" s="26">
+      <c r="B3" s="25">
         <v>9.7299999999999998E-2</v>
       </c>
-      <c r="C3" s="26">
+      <c r="C3" s="25">
         <v>0.34429999999999999</v>
       </c>
-      <c r="D3" s="26">
+      <c r="D3" s="25">
         <v>0.16300000000000001</v>
       </c>
-      <c r="E3" s="26">
+      <c r="E3" s="25">
         <v>0.36749999999999999</v>
       </c>
-      <c r="F3" s="26">
+      <c r="F3" s="25">
         <v>1.9300000000000001E-2</v>
       </c>
-      <c r="G3" s="26">
+      <c r="G3" s="25">
         <v>1.47E-2</v>
       </c>
     </row>
@@ -14683,22 +14886,22 @@
       <c r="A4" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="B4" s="21">
+      <c r="B4" s="20">
         <v>0.25</v>
       </c>
-      <c r="C4" s="21">
+      <c r="C4" s="20">
         <v>0.53</v>
       </c>
-      <c r="D4" s="21">
+      <c r="D4" s="20">
         <v>1.45</v>
       </c>
-      <c r="E4" s="21">
+      <c r="E4" s="20">
         <v>1.52</v>
       </c>
-      <c r="F4" s="21">
+      <c r="F4" s="20">
         <v>1.4</v>
       </c>
-      <c r="G4" s="21">
+      <c r="G4" s="20">
         <v>1.39</v>
       </c>
     </row>
@@ -14706,22 +14909,22 @@
       <c r="A5" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="B5" s="26">
+      <c r="B5" s="25">
         <v>9.8900000000000002E-2</v>
       </c>
-      <c r="C5" s="26">
+      <c r="C5" s="25">
         <v>0.15190000000000001</v>
       </c>
-      <c r="D5" s="26">
+      <c r="D5" s="25">
         <v>0.3422</v>
       </c>
-      <c r="E5" s="26">
+      <c r="E5" s="25">
         <v>0.26300000000000001</v>
       </c>
-      <c r="F5" s="26">
+      <c r="F5" s="25">
         <v>0.2402</v>
       </c>
-      <c r="G5" s="26">
+      <c r="G5" s="25">
         <v>0.24310000000000001</v>
       </c>
     </row>
@@ -14729,22 +14932,22 @@
       <c r="A6" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="B6" s="21">
+      <c r="B6" s="20">
         <v>0.72</v>
       </c>
-      <c r="C6" s="21">
+      <c r="C6" s="20">
         <v>0.74</v>
       </c>
-      <c r="D6" s="21">
+      <c r="D6" s="20">
         <v>2.0499999999999998</v>
       </c>
-      <c r="E6" s="21">
+      <c r="E6" s="20">
         <v>2.15</v>
       </c>
-      <c r="F6" s="21">
+      <c r="F6" s="20">
         <v>1.98</v>
       </c>
-      <c r="G6" s="21">
+      <c r="G6" s="20">
         <v>1.96</v>
       </c>
     </row>
@@ -14752,22 +14955,22 @@
       <c r="A7" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="B7" s="21">
+      <c r="B7" s="20">
         <v>0.68</v>
       </c>
-      <c r="C7" s="21">
+      <c r="C7" s="20">
         <v>0.73</v>
       </c>
-      <c r="D7" s="21">
+      <c r="D7" s="20">
         <v>2</v>
       </c>
-      <c r="E7" s="21">
+      <c r="E7" s="20">
         <v>2.1</v>
       </c>
-      <c r="F7" s="21">
+      <c r="F7" s="20">
         <v>1.94</v>
       </c>
-      <c r="G7" s="21">
+      <c r="G7" s="20">
         <v>1.92</v>
       </c>
     </row>
@@ -14775,22 +14978,22 @@
       <c r="A8" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="B8" s="21">
+      <c r="B8" s="20">
         <v>1.32</v>
       </c>
-      <c r="C8" s="21">
+      <c r="C8" s="20">
         <v>2.76</v>
       </c>
-      <c r="D8" s="21">
+      <c r="D8" s="20">
         <v>0.66</v>
       </c>
-      <c r="E8" s="21">
+      <c r="E8" s="20">
         <v>2.21</v>
       </c>
-      <c r="F8" s="21">
+      <c r="F8" s="20">
         <v>2.2000000000000002</v>
       </c>
-      <c r="G8" s="21">
+      <c r="G8" s="20">
         <v>2.39</v>
       </c>
     </row>
@@ -14853,22 +15056,22 @@
       <c r="A12" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="B12" s="21">
+      <c r="B12" s="20">
         <v>93.05</v>
       </c>
-      <c r="C12" s="21">
+      <c r="C12" s="20">
         <v>136.35</v>
       </c>
-      <c r="D12" s="21">
+      <c r="D12" s="20">
         <v>152.30000000000001</v>
       </c>
-      <c r="E12" s="21">
+      <c r="E12" s="20">
         <v>142.13</v>
       </c>
-      <c r="F12" s="21">
+      <c r="F12" s="20">
         <v>140.59</v>
       </c>
-      <c r="G12" s="21">
+      <c r="G12" s="20">
         <v>141.96</v>
       </c>
     </row>
@@ -14876,22 +15079,22 @@
       <c r="A13" s="7" t="s">
         <v>27</v>
       </c>
-      <c r="B13" s="21">
+      <c r="B13" s="20">
         <v>86.72</v>
       </c>
-      <c r="C13" s="21">
+      <c r="C13" s="20">
         <v>129.49</v>
       </c>
-      <c r="D13" s="21">
+      <c r="D13" s="20">
         <v>144.18</v>
       </c>
-      <c r="E13" s="21">
+      <c r="E13" s="20">
         <v>132.56</v>
       </c>
-      <c r="F13" s="21">
+      <c r="F13" s="20">
         <v>129.03</v>
       </c>
-      <c r="G13" s="21">
+      <c r="G13" s="20">
         <v>129.96</v>
       </c>
     </row>
@@ -14899,22 +15102,22 @@
       <c r="A14" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="B14" s="21">
+      <c r="B14" s="20">
         <v>82.26</v>
       </c>
-      <c r="C14" s="21">
+      <c r="C14" s="20">
         <v>123.76</v>
       </c>
-      <c r="D14" s="21">
+      <c r="D14" s="20">
         <v>132.85</v>
       </c>
-      <c r="E14" s="21">
+      <c r="E14" s="20">
         <v>124.02</v>
       </c>
-      <c r="F14" s="21">
+      <c r="F14" s="20">
         <v>121.34</v>
       </c>
-      <c r="G14" s="21">
+      <c r="G14" s="20">
         <v>120.17</v>
       </c>
     </row>
@@ -14922,22 +15125,22 @@
       <c r="A15" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="B15" s="21">
+      <c r="B15" s="20">
         <v>6.33</v>
       </c>
-      <c r="C15" s="21">
+      <c r="C15" s="20">
         <v>6.86</v>
       </c>
-      <c r="D15" s="21">
+      <c r="D15" s="20">
         <v>8.1199999999999992</v>
       </c>
-      <c r="E15" s="21">
+      <c r="E15" s="20">
         <v>9.57</v>
       </c>
-      <c r="F15" s="21">
+      <c r="F15" s="20">
         <v>11.56</v>
       </c>
-      <c r="G15" s="21">
+      <c r="G15" s="20">
         <v>11.99</v>
       </c>
     </row>
@@ -14945,22 +15148,22 @@
       <c r="A16" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="B16" s="21">
+      <c r="B16" s="20">
         <v>8.98</v>
       </c>
-      <c r="C16" s="21">
+      <c r="C16" s="20">
         <v>21.77</v>
       </c>
-      <c r="D16" s="21">
+      <c r="D16" s="20">
         <v>15.43</v>
       </c>
-      <c r="E16" s="21">
+      <c r="E16" s="20">
         <v>11.2</v>
       </c>
-      <c r="F16" s="21">
+      <c r="F16" s="20">
         <v>8.99</v>
       </c>
-      <c r="G16" s="21">
+      <c r="G16" s="20">
         <v>8.61</v>
       </c>
     </row>
@@ -14968,22 +15171,22 @@
       <c r="A17" s="5" t="s">
         <v>42</v>
       </c>
-      <c r="B17" s="21">
+      <c r="B17" s="20">
         <v>421.18</v>
       </c>
-      <c r="C17" s="21">
+      <c r="C17" s="20">
         <v>705.54</v>
       </c>
-      <c r="D17" s="21">
+      <c r="D17" s="20">
         <v>705.56</v>
       </c>
-      <c r="E17" s="21">
+      <c r="E17" s="20">
         <v>707.59</v>
       </c>
-      <c r="F17" s="21">
+      <c r="F17" s="20">
         <v>709.74</v>
       </c>
-      <c r="G17" s="21">
+      <c r="G17" s="20">
         <v>707.79</v>
       </c>
     </row>
@@ -14991,22 +15194,22 @@
       <c r="A18" s="9" t="s">
         <v>33</v>
       </c>
-      <c r="B18" s="21">
+      <c r="B18" s="20">
         <v>8.77</v>
       </c>
-      <c r="C18" s="21">
+      <c r="C18" s="20">
         <v>9.49</v>
       </c>
-      <c r="D18" s="21">
+      <c r="D18" s="20">
         <v>11.23</v>
       </c>
-      <c r="E18" s="21">
+      <c r="E18" s="20">
         <v>13.24</v>
       </c>
-      <c r="F18" s="21">
+      <c r="F18" s="20">
         <v>16.04</v>
       </c>
-      <c r="G18" s="21">
+      <c r="G18" s="20">
         <v>16.64</v>
       </c>
     </row>
@@ -15014,22 +15217,22 @@
       <c r="A19" s="9" t="s">
         <v>34</v>
       </c>
-      <c r="B19" s="21">
+      <c r="B19" s="20">
         <v>12.99</v>
       </c>
-      <c r="C19" s="21">
+      <c r="C19" s="20">
         <v>18.04</v>
       </c>
-      <c r="D19" s="21">
+      <c r="D19" s="20">
         <v>16.36</v>
       </c>
-      <c r="E19" s="21">
+      <c r="E19" s="20">
         <v>12.96</v>
       </c>
-      <c r="F19" s="21">
+      <c r="F19" s="20">
         <v>10.49</v>
       </c>
-      <c r="G19" s="21">
+      <c r="G19" s="20">
         <v>10.02</v>
       </c>
     </row>
@@ -15069,22 +15272,22 @@
       <c r="A22" s="5" t="s">
         <v>36</v>
       </c>
-      <c r="B22" s="21">
+      <c r="B22" s="20">
         <v>-0.63</v>
       </c>
-      <c r="C22" s="21">
+      <c r="C22" s="20">
         <v>1.26</v>
       </c>
-      <c r="D22" s="21">
+      <c r="D22" s="20">
         <v>12.79</v>
       </c>
-      <c r="E22" s="21">
+      <c r="E22" s="20">
         <v>-3.42</v>
       </c>
-      <c r="F22" s="21">
+      <c r="F22" s="20">
         <v>-2.5</v>
       </c>
-      <c r="G22" s="21">
+      <c r="G22" s="20">
         <v>-2.5</v>
       </c>
     </row>
@@ -15092,22 +15295,22 @@
       <c r="A23" s="5" t="s">
         <v>37</v>
       </c>
-      <c r="B23" s="21">
+      <c r="B23" s="20">
         <v>-0.22</v>
       </c>
-      <c r="C23" s="21">
+      <c r="C23" s="20">
         <v>-0.74</v>
       </c>
-      <c r="D23" s="21">
+      <c r="D23" s="20">
         <v>-0.02</v>
       </c>
-      <c r="E23" s="21">
+      <c r="E23" s="20">
         <v>-0.31</v>
       </c>
-      <c r="F23" s="21">
+      <c r="F23" s="20">
         <v>-0.22</v>
       </c>
-      <c r="G23" s="21">
+      <c r="G23" s="20">
         <v>-0.22</v>
       </c>
     </row>
@@ -15115,22 +15318,22 @@
       <c r="A24" s="5" t="s">
         <v>38</v>
       </c>
-      <c r="B24" s="21">
+      <c r="B24" s="20">
         <v>0.77</v>
       </c>
-      <c r="C24" s="21">
+      <c r="C24" s="20">
         <v>-0.06</v>
       </c>
-      <c r="D24" s="21">
+      <c r="D24" s="20">
         <v>-0.09</v>
       </c>
-      <c r="E24" s="21">
+      <c r="E24" s="20">
         <v>-0.18</v>
       </c>
-      <c r="F24" s="21">
+      <c r="F24" s="20">
         <v>0.51</v>
       </c>
-      <c r="G24" s="21">
+      <c r="G24" s="20">
         <v>0.51</v>
       </c>
     </row>
@@ -15138,22 +15341,22 @@
       <c r="A25" s="5" t="s">
         <v>40</v>
       </c>
-      <c r="B25" s="21">
+      <c r="B25" s="20">
         <v>0.81</v>
       </c>
-      <c r="C25" s="21">
+      <c r="C25" s="20">
         <v>1.05</v>
       </c>
-      <c r="D25" s="21">
+      <c r="D25" s="20">
         <v>1.53</v>
       </c>
-      <c r="E25" s="21">
+      <c r="E25" s="20">
         <v>2.72</v>
       </c>
-      <c r="F25" s="21">
+      <c r="F25" s="20">
         <v>2.66</v>
       </c>
-      <c r="G25" s="21">
+      <c r="G25" s="20">
         <v>2.66</v>
       </c>
     </row>
@@ -15161,22 +15364,22 @@
       <c r="A26" s="5" t="s">
         <v>41</v>
       </c>
-      <c r="B26" s="21">
+      <c r="B26" s="20">
         <v>-0.09</v>
       </c>
-      <c r="C26" s="21">
+      <c r="C26" s="20">
         <v>0.46</v>
       </c>
-      <c r="D26" s="21">
+      <c r="D26" s="20">
         <v>12.69</v>
       </c>
-      <c r="E26" s="21">
+      <c r="E26" s="20">
         <v>-3.91</v>
       </c>
-      <c r="F26" s="21">
+      <c r="F26" s="20">
         <v>-2.2000000000000002</v>
       </c>
-      <c r="G26" s="21">
+      <c r="G26" s="20">
         <v>-2.2000000000000002</v>
       </c>
     </row>
@@ -15189,7 +15392,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D182C88B-880A-4B87-AD8A-FBBFB305FA84}">
   <dimension ref="A1:G36"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B1" sqref="B1:G37"/>
     </sheetView>
   </sheetViews>
@@ -15228,22 +15431,22 @@
       <c r="A2" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="B2" s="21">
+      <c r="B2" s="20">
         <v>3.22</v>
       </c>
-      <c r="C2" s="21">
+      <c r="C2" s="20">
         <v>3.22</v>
       </c>
-      <c r="D2" s="21">
+      <c r="D2" s="20">
         <v>3.45</v>
       </c>
-      <c r="E2" s="21">
+      <c r="E2" s="20">
         <v>4</v>
       </c>
-      <c r="F2" s="21">
+      <c r="F2" s="20">
         <v>4.32</v>
       </c>
-      <c r="G2" s="21">
+      <c r="G2" s="20">
         <v>4.3099999999999996</v>
       </c>
     </row>
@@ -15251,22 +15454,22 @@
       <c r="A3" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="B3" s="26">
+      <c r="B3" s="25">
         <v>0.1211</v>
       </c>
-      <c r="C3" s="26">
+      <c r="C3" s="25">
         <v>2.9999999999999997E-4</v>
       </c>
-      <c r="D3" s="26">
+      <c r="D3" s="25">
         <v>6.9199999999999998E-2</v>
       </c>
-      <c r="E3" s="26">
+      <c r="E3" s="25">
         <v>0.15959999999999999</v>
       </c>
-      <c r="F3" s="26">
+      <c r="F3" s="25">
         <v>8.0600000000000005E-2</v>
       </c>
-      <c r="G3" s="26">
+      <c r="G3" s="25">
         <v>-1E-3</v>
       </c>
     </row>
@@ -15274,22 +15477,22 @@
       <c r="A4" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="B4" s="21">
+      <c r="B4" s="20">
         <v>2.0299999999999998</v>
       </c>
-      <c r="C4" s="21">
+      <c r="C4" s="20">
         <v>2.0499999999999998</v>
       </c>
-      <c r="D4" s="21">
+      <c r="D4" s="20">
         <v>2.09</v>
       </c>
-      <c r="E4" s="21">
+      <c r="E4" s="20">
         <v>2.36</v>
       </c>
-      <c r="F4" s="21">
+      <c r="F4" s="20">
         <v>2.75</v>
       </c>
-      <c r="G4" s="21">
+      <c r="G4" s="20">
         <v>2.82</v>
       </c>
     </row>
@@ -15297,22 +15500,22 @@
       <c r="A5" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="B5" s="26">
+      <c r="B5" s="25">
         <v>0.63049999999999995</v>
       </c>
-      <c r="C5" s="26">
+      <c r="C5" s="25">
         <v>0.63639999999999997</v>
       </c>
-      <c r="D5" s="26">
+      <c r="D5" s="25">
         <v>0.6069</v>
       </c>
-      <c r="E5" s="26">
+      <c r="E5" s="25">
         <v>0.5917</v>
       </c>
-      <c r="F5" s="26">
+      <c r="F5" s="25">
         <v>0.63700000000000001</v>
       </c>
-      <c r="G5" s="26">
+      <c r="G5" s="25">
         <v>0.65410000000000001</v>
       </c>
     </row>
@@ -15320,22 +15523,22 @@
       <c r="A6" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="B6" s="21">
+      <c r="B6" s="20">
         <v>0.47</v>
       </c>
-      <c r="C6" s="21">
+      <c r="C6" s="20">
         <v>0.52</v>
       </c>
-      <c r="D6" s="21">
+      <c r="D6" s="20">
         <v>0.53</v>
       </c>
-      <c r="E6" s="21">
+      <c r="E6" s="20">
         <v>0.61</v>
       </c>
-      <c r="F6" s="21">
+      <c r="F6" s="20">
         <v>0.98</v>
       </c>
-      <c r="G6" s="21">
+      <c r="G6" s="20">
         <v>0.99</v>
       </c>
     </row>
@@ -15343,22 +15546,22 @@
       <c r="A7" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="B7" s="26">
+      <c r="B7" s="25">
         <v>0.14449999999999999</v>
       </c>
-      <c r="C7" s="26">
+      <c r="C7" s="25">
         <v>0.16020000000000001</v>
       </c>
-      <c r="D7" s="26">
+      <c r="D7" s="25">
         <v>0.155</v>
       </c>
-      <c r="E7" s="26">
+      <c r="E7" s="25">
         <v>0.15310000000000001</v>
       </c>
-      <c r="F7" s="26">
+      <c r="F7" s="25">
         <v>0.22589999999999999</v>
       </c>
-      <c r="G7" s="26">
+      <c r="G7" s="25">
         <v>0.2296</v>
       </c>
     </row>
@@ -15366,22 +15569,22 @@
       <c r="A8" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="B8" s="21">
+      <c r="B8" s="20">
         <v>0.52</v>
       </c>
-      <c r="C8" s="21">
+      <c r="C8" s="20">
         <v>0.73</v>
       </c>
-      <c r="D8" s="21">
+      <c r="D8" s="20">
         <v>0.66</v>
       </c>
-      <c r="E8" s="21">
+      <c r="E8" s="20">
         <v>0.59</v>
       </c>
-      <c r="F8" s="21">
+      <c r="F8" s="20">
         <v>1.1299999999999999</v>
       </c>
-      <c r="G8" s="21">
+      <c r="G8" s="20">
         <v>1.05</v>
       </c>
     </row>
@@ -15389,22 +15592,22 @@
       <c r="A9" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="B9" s="26">
+      <c r="B9" s="25">
         <v>0.161</v>
       </c>
-      <c r="C9" s="26">
+      <c r="C9" s="25">
         <v>0.2278</v>
       </c>
-      <c r="D9" s="26">
+      <c r="D9" s="25">
         <v>0.19209999999999999</v>
       </c>
-      <c r="E9" s="26">
+      <c r="E9" s="25">
         <v>0.14710000000000001</v>
       </c>
-      <c r="F9" s="26">
+      <c r="F9" s="25">
         <v>0.26269999999999999</v>
       </c>
-      <c r="G9" s="26">
+      <c r="G9" s="25">
         <v>0.24349999999999999</v>
       </c>
     </row>
@@ -15412,22 +15615,22 @@
       <c r="A10" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="B10" s="21">
+      <c r="B10" s="20">
         <v>0.78</v>
       </c>
-      <c r="C10" s="21">
+      <c r="C10" s="20">
         <v>0.99</v>
       </c>
-      <c r="D10" s="21">
+      <c r="D10" s="20">
         <v>0.91</v>
       </c>
-      <c r="E10" s="21">
+      <c r="E10" s="20">
         <v>0.98</v>
       </c>
-      <c r="F10" s="21">
+      <c r="F10" s="20">
         <v>1.38</v>
       </c>
-      <c r="G10" s="21">
+      <c r="G10" s="20">
         <v>1.32</v>
       </c>
     </row>
@@ -15435,22 +15638,22 @@
       <c r="A11" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="B11" s="26">
+      <c r="B11" s="25">
         <v>0.2417</v>
       </c>
-      <c r="C11" s="26">
+      <c r="C11" s="25">
         <v>0.30640000000000001</v>
       </c>
-      <c r="D11" s="26">
+      <c r="D11" s="25">
         <v>0.26440000000000002</v>
       </c>
-      <c r="E11" s="26">
+      <c r="E11" s="25">
         <v>0.2445</v>
       </c>
-      <c r="F11" s="26">
+      <c r="F11" s="25">
         <v>0.32019999999999998</v>
       </c>
-      <c r="G11" s="26">
+      <c r="G11" s="25">
         <v>0.30669999999999997</v>
       </c>
     </row>
@@ -15458,22 +15661,22 @@
       <c r="A12" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="B12" s="21">
+      <c r="B12" s="20">
         <v>0.39</v>
       </c>
-      <c r="C12" s="21">
+      <c r="C12" s="20">
         <v>0.56000000000000005</v>
       </c>
-      <c r="D12" s="21">
+      <c r="D12" s="20">
         <v>0.54</v>
       </c>
-      <c r="E12" s="21">
+      <c r="E12" s="20">
         <v>0.46</v>
       </c>
-      <c r="F12" s="21">
+      <c r="F12" s="20">
         <v>0.97</v>
       </c>
-      <c r="G12" s="21">
+      <c r="G12" s="20">
         <v>0.94</v>
       </c>
     </row>
@@ -15481,22 +15684,22 @@
       <c r="A13" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="B13" s="26">
+      <c r="B13" s="25">
         <v>0.1198</v>
       </c>
-      <c r="C13" s="26">
+      <c r="C13" s="25">
         <v>0.1739</v>
       </c>
-      <c r="D13" s="26">
+      <c r="D13" s="25">
         <v>0.15740000000000001</v>
       </c>
-      <c r="E13" s="26">
+      <c r="E13" s="25">
         <v>0.1148</v>
       </c>
-      <c r="F13" s="26">
+      <c r="F13" s="25">
         <v>0.22389999999999999</v>
       </c>
-      <c r="G13" s="26">
+      <c r="G13" s="25">
         <v>0.2185</v>
       </c>
     </row>
@@ -15504,22 +15707,22 @@
       <c r="A14" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="B14" s="21">
+      <c r="B14" s="20">
         <v>1.88</v>
       </c>
-      <c r="C14" s="21">
+      <c r="C14" s="20">
         <v>2.72</v>
       </c>
-      <c r="D14" s="21">
+      <c r="D14" s="20">
         <v>2.82</v>
       </c>
-      <c r="E14" s="21">
+      <c r="E14" s="20">
         <v>2.46</v>
       </c>
-      <c r="F14" s="21">
+      <c r="F14" s="20">
         <v>5.22</v>
       </c>
-      <c r="G14" s="21">
+      <c r="G14" s="20">
         <v>5.14</v>
       </c>
     </row>
@@ -15527,22 +15730,22 @@
       <c r="A15" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="B15" s="21">
+      <c r="B15" s="20">
         <v>1.88</v>
       </c>
-      <c r="C15" s="21">
+      <c r="C15" s="20">
         <v>2.72</v>
       </c>
-      <c r="D15" s="21">
+      <c r="D15" s="20">
         <v>2.82</v>
       </c>
-      <c r="E15" s="21">
+      <c r="E15" s="20">
         <v>2.44</v>
       </c>
-      <c r="F15" s="21">
+      <c r="F15" s="20">
         <v>5.22</v>
       </c>
-      <c r="G15" s="21">
+      <c r="G15" s="20">
         <v>5.0999999999999996</v>
       </c>
     </row>
@@ -15550,22 +15753,22 @@
       <c r="A16" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="B16" s="21">
+      <c r="B16" s="20">
         <v>1.76</v>
       </c>
-      <c r="C16" s="21">
+      <c r="C16" s="20">
         <v>2.31</v>
       </c>
-      <c r="D16" s="21">
+      <c r="D16" s="20">
         <v>2.5099999999999998</v>
       </c>
-      <c r="E16" s="21">
+      <c r="E16" s="20">
         <v>3.14</v>
       </c>
-      <c r="F16" s="21">
+      <c r="F16" s="20">
         <v>5.25</v>
       </c>
-      <c r="G16" s="21">
+      <c r="G16" s="20">
         <v>4.8099999999999996</v>
       </c>
     </row>
@@ -15573,22 +15776,22 @@
       <c r="A17" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="B17" s="21">
+      <c r="B17" s="20">
         <v>0.13</v>
       </c>
-      <c r="C17" s="21">
+      <c r="C17" s="20">
         <v>0.15</v>
       </c>
-      <c r="D17" s="21">
+      <c r="D17" s="20">
         <v>1</v>
       </c>
-      <c r="E17" s="21">
+      <c r="E17" s="20">
         <v>0.4</v>
       </c>
-      <c r="F17" s="21">
+      <c r="F17" s="20">
         <v>0.45</v>
       </c>
-      <c r="G17" s="21">
+      <c r="G17" s="20">
         <v>0.6</v>
       </c>
     </row>
@@ -15628,22 +15831,22 @@
       <c r="A20" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="B20" s="21">
+      <c r="B20" s="20">
         <v>6.4</v>
       </c>
-      <c r="C20" s="21">
+      <c r="C20" s="20">
         <v>6.39</v>
       </c>
-      <c r="D20" s="21">
+      <c r="D20" s="20">
         <v>6.92</v>
       </c>
-      <c r="E20" s="21">
+      <c r="E20" s="20">
         <v>7.5</v>
       </c>
-      <c r="F20" s="21">
+      <c r="F20" s="20">
         <v>7.62</v>
       </c>
-      <c r="G20" s="21">
+      <c r="G20" s="20">
         <v>7.62</v>
       </c>
     </row>
@@ -15651,22 +15854,22 @@
       <c r="A21" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="B21" s="21">
+      <c r="B21" s="20">
         <v>2.71</v>
       </c>
-      <c r="C21" s="21">
+      <c r="C21" s="20">
         <v>2.78</v>
       </c>
-      <c r="D21" s="21">
+      <c r="D21" s="20">
         <v>2.5499999999999998</v>
       </c>
-      <c r="E21" s="21">
+      <c r="E21" s="20">
         <v>2.59</v>
       </c>
-      <c r="F21" s="21">
+      <c r="F21" s="20">
         <v>1.98</v>
       </c>
-      <c r="G21" s="21">
+      <c r="G21" s="20">
         <v>1.98</v>
       </c>
     </row>
@@ -15674,22 +15877,22 @@
       <c r="A22" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="B22" s="21">
+      <c r="B22" s="20">
         <v>1.37</v>
       </c>
-      <c r="C22" s="21">
+      <c r="C22" s="20">
         <v>1.32</v>
       </c>
-      <c r="D22" s="21">
+      <c r="D22" s="20">
         <v>1.22</v>
       </c>
-      <c r="E22" s="21">
+      <c r="E22" s="20">
         <v>1.29</v>
       </c>
-      <c r="F22" s="21">
+      <c r="F22" s="20">
         <v>0.69</v>
       </c>
-      <c r="G22" s="21">
+      <c r="G22" s="20">
         <v>0.69</v>
       </c>
     </row>
@@ -15697,22 +15900,22 @@
       <c r="A23" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="B23" s="21">
+      <c r="B23" s="20">
         <v>3.69</v>
       </c>
-      <c r="C23" s="21">
+      <c r="C23" s="20">
         <v>3.6</v>
       </c>
-      <c r="D23" s="21">
+      <c r="D23" s="20">
         <v>4.38</v>
       </c>
-      <c r="E23" s="21">
+      <c r="E23" s="20">
         <v>4.91</v>
       </c>
-      <c r="F23" s="21">
+      <c r="F23" s="20">
         <v>5.63</v>
       </c>
-      <c r="G23" s="21">
+      <c r="G23" s="20">
         <v>5.63</v>
       </c>
     </row>
@@ -15720,22 +15923,22 @@
       <c r="A24" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="B24" s="21">
+      <c r="B24" s="20">
         <v>0.84</v>
       </c>
-      <c r="C24" s="21">
+      <c r="C24" s="20">
         <v>1.22</v>
       </c>
-      <c r="D24" s="21">
+      <c r="D24" s="20">
         <v>1.2</v>
       </c>
-      <c r="E24" s="21">
+      <c r="E24" s="20">
         <v>1.34</v>
       </c>
-      <c r="F24" s="21">
+      <c r="F24" s="20">
         <v>1.1200000000000001</v>
       </c>
-      <c r="G24" s="21">
+      <c r="G24" s="20">
         <v>1.1200000000000001</v>
       </c>
     </row>
@@ -15743,22 +15946,22 @@
       <c r="A25" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="B25" s="21">
+      <c r="B25" s="20">
         <v>1.32</v>
       </c>
-      <c r="C25" s="21">
+      <c r="C25" s="20">
         <v>1.5</v>
       </c>
-      <c r="D25" s="21">
+      <c r="D25" s="20">
         <v>1.57</v>
       </c>
-      <c r="E25" s="21">
+      <c r="E25" s="20">
         <v>1.54</v>
       </c>
-      <c r="F25" s="21">
+      <c r="F25" s="20">
         <v>1.96</v>
       </c>
-      <c r="G25" s="21">
+      <c r="G25" s="20">
         <v>1.96</v>
       </c>
     </row>
@@ -15766,22 +15969,22 @@
       <c r="A26" s="5" t="s">
         <v>42</v>
       </c>
-      <c r="B26" s="21">
+      <c r="B26" s="20">
         <v>205.3</v>
       </c>
-      <c r="C26" s="21">
+      <c r="C26" s="20">
         <v>205.52</v>
       </c>
-      <c r="D26" s="21">
+      <c r="D26" s="20">
         <v>192.13</v>
       </c>
-      <c r="E26" s="21">
+      <c r="E26" s="20">
         <v>185.13</v>
       </c>
-      <c r="F26" s="21">
+      <c r="F26" s="20">
         <v>185.13</v>
       </c>
-      <c r="G26" s="21">
+      <c r="G26" s="20">
         <v>181.07</v>
       </c>
     </row>
@@ -15789,22 +15992,22 @@
       <c r="A27" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="B27" s="21">
+      <c r="B27" s="20">
         <v>17.89</v>
       </c>
-      <c r="C27" s="21">
+      <c r="C27" s="20">
         <v>17.5</v>
       </c>
-      <c r="D27" s="21">
+      <c r="D27" s="20">
         <v>22.74</v>
       </c>
-      <c r="E27" s="21">
+      <c r="E27" s="20">
         <v>26.5</v>
       </c>
-      <c r="F27" s="21">
+      <c r="F27" s="20">
         <v>30.39</v>
       </c>
-      <c r="G27" s="21">
+      <c r="G27" s="20">
         <v>30.39</v>
       </c>
     </row>
@@ -15812,22 +16015,22 @@
       <c r="A28" s="5" t="s">
         <v>34</v>
       </c>
-      <c r="B28" s="21">
+      <c r="B28" s="20">
         <v>0.37</v>
       </c>
-      <c r="C28" s="21">
+      <c r="C28" s="20">
         <v>0.37</v>
       </c>
-      <c r="D28" s="21">
+      <c r="D28" s="20">
         <v>0.28000000000000003</v>
       </c>
-      <c r="E28" s="21">
+      <c r="E28" s="20">
         <v>0.26</v>
       </c>
-      <c r="F28" s="21">
+      <c r="F28" s="20">
         <v>0.12</v>
       </c>
-      <c r="G28" s="21">
+      <c r="G28" s="20">
         <v>0.12</v>
       </c>
     </row>
@@ -15867,22 +16070,22 @@
       <c r="A31" s="5" t="s">
         <v>36</v>
       </c>
-      <c r="B31" s="21">
+      <c r="B31" s="20">
         <v>0.57999999999999996</v>
       </c>
-      <c r="C31" s="21">
+      <c r="C31" s="20">
         <v>0.59</v>
       </c>
-      <c r="D31" s="21">
+      <c r="D31" s="20">
         <v>0.59</v>
       </c>
-      <c r="E31" s="21">
+      <c r="E31" s="20">
         <v>0.39</v>
       </c>
-      <c r="F31" s="21">
+      <c r="F31" s="20">
         <v>0.82</v>
       </c>
-      <c r="G31" s="21">
+      <c r="G31" s="20">
         <v>0.93</v>
       </c>
     </row>
@@ -15890,22 +16093,22 @@
       <c r="A32" s="5" t="s">
         <v>37</v>
       </c>
-      <c r="B32" s="21">
+      <c r="B32" s="20">
         <v>-0.22</v>
       </c>
-      <c r="C32" s="21">
+      <c r="C32" s="20">
         <v>-0.01</v>
       </c>
-      <c r="D32" s="21">
+      <c r="D32" s="20">
         <v>-0.33</v>
       </c>
-      <c r="E32" s="21">
+      <c r="E32" s="20">
         <v>-0.14000000000000001</v>
       </c>
-      <c r="F32" s="21">
+      <c r="F32" s="20">
         <v>-0.3</v>
       </c>
-      <c r="G32" s="21">
+      <c r="G32" s="20">
         <v>-0.24</v>
       </c>
     </row>
@@ -15913,22 +16116,22 @@
       <c r="A33" s="5" t="s">
         <v>38</v>
       </c>
-      <c r="B33" s="21">
+      <c r="B33" s="20">
         <v>0.03</v>
       </c>
-      <c r="C33" s="21">
+      <c r="C33" s="20">
         <v>-0.13</v>
       </c>
-      <c r="D33" s="21">
+      <c r="D33" s="20">
         <v>-0.33</v>
       </c>
-      <c r="E33" s="21">
+      <c r="E33" s="20">
         <v>-0.15</v>
       </c>
-      <c r="F33" s="21">
+      <c r="F33" s="20">
         <v>-0.71</v>
       </c>
-      <c r="G33" s="21">
+      <c r="G33" s="20">
         <v>-0.41</v>
       </c>
     </row>
@@ -15936,22 +16139,22 @@
       <c r="A34" s="5" t="s">
         <v>39</v>
       </c>
-      <c r="B34" s="21">
+      <c r="B34" s="20">
         <v>0.26</v>
       </c>
-      <c r="C34" s="21">
+      <c r="C34" s="20">
         <v>0.23</v>
       </c>
-      <c r="D34" s="21">
+      <c r="D34" s="20">
         <v>0.21</v>
       </c>
-      <c r="E34" s="21">
+      <c r="E34" s="20">
         <v>0.27</v>
       </c>
-      <c r="F34" s="21">
+      <c r="F34" s="20">
         <v>0.3</v>
       </c>
-      <c r="G34" s="21">
+      <c r="G34" s="20">
         <v>0.45</v>
       </c>
     </row>
@@ -15959,22 +16162,22 @@
       <c r="A35" s="5" t="s">
         <v>40</v>
       </c>
-      <c r="B35" s="21">
+      <c r="B35" s="20">
         <v>0.36</v>
       </c>
-      <c r="C35" s="21">
+      <c r="C35" s="20">
         <v>0.38</v>
       </c>
-      <c r="D35" s="21">
+      <c r="D35" s="20">
         <v>0.36</v>
       </c>
-      <c r="E35" s="21">
+      <c r="E35" s="20">
         <v>0.41</v>
       </c>
-      <c r="F35" s="21">
+      <c r="F35" s="20">
         <v>0.64</v>
       </c>
-      <c r="G35" s="21">
+      <c r="G35" s="20">
         <v>0.55000000000000004</v>
       </c>
     </row>
@@ -15982,22 +16185,22 @@
       <c r="A36" s="5" t="s">
         <v>41</v>
       </c>
-      <c r="B36" s="21">
+      <c r="B36" s="20">
         <v>0.39</v>
       </c>
-      <c r="C36" s="21">
+      <c r="C36" s="20">
         <v>0.45</v>
       </c>
-      <c r="D36" s="21">
+      <c r="D36" s="20">
         <v>-7.0000000000000007E-2</v>
       </c>
-      <c r="E36" s="21">
+      <c r="E36" s="20">
         <v>0.1</v>
       </c>
-      <c r="F36" s="21">
+      <c r="F36" s="20">
         <v>-0.19</v>
       </c>
-      <c r="G36" s="21">
+      <c r="G36" s="20">
         <v>0.28000000000000003</v>
       </c>
     </row>
@@ -16010,18 +16213,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{54171494-C811-4F19-A37C-A35AC15A1124}">
   <dimension ref="A1:M36"/>
   <sheetViews>
-    <sheetView topLeftCell="A5" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="M27" sqref="M27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
-    <col min="1" max="1" width="36.83984375" style="14" bestFit="1" customWidth="1"/>
-    <col min="2" max="4" width="7.83984375" style="14" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="8.89453125" style="14" customWidth="1"/>
-    <col min="6" max="6" width="8.89453125" style="14" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="11.1015625" style="14" bestFit="1" customWidth="1"/>
-    <col min="8" max="16384" width="8.83984375" style="14"/>
+    <col min="1" max="1" width="36.83984375" bestFit="1" customWidth="1"/>
+    <col min="2" max="4" width="7.83984375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="8.89453125" customWidth="1"/>
+    <col min="6" max="6" width="8.89453125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11.1015625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="15.6" x14ac:dyDescent="0.6">
@@ -16048,382 +16250,382 @@
       </c>
     </row>
     <row r="2" spans="1:8" ht="15.6" x14ac:dyDescent="0.6">
-      <c r="A2" s="15" t="s">
+      <c r="A2" s="14" t="s">
         <v>8</v>
       </c>
-      <c r="B2" s="21">
+      <c r="B2" s="20">
         <v>16.68</v>
       </c>
-      <c r="C2" s="21">
+      <c r="C2" s="20">
         <v>26.91</v>
       </c>
-      <c r="D2" s="21">
+      <c r="D2" s="20">
         <v>26.97</v>
       </c>
-      <c r="E2" s="21">
+      <c r="E2" s="20">
         <v>60.92</v>
       </c>
-      <c r="F2" s="21">
+      <c r="F2" s="20">
         <v>130.5</v>
       </c>
-      <c r="G2" s="21">
+      <c r="G2" s="20">
         <v>148.52000000000001</v>
       </c>
     </row>
     <row r="3" spans="1:8" ht="15.6" x14ac:dyDescent="0.6">
-      <c r="A3" s="16" t="s">
+      <c r="A3" s="15" t="s">
         <v>9</v>
       </c>
-      <c r="B3" s="27">
+      <c r="B3" s="26">
         <v>0.52729999999999999</v>
       </c>
-      <c r="C3" s="27">
+      <c r="C3" s="26">
         <v>0.61399999999999999</v>
       </c>
-      <c r="D3" s="27">
+      <c r="D3" s="26">
         <v>2.2000000000000001E-3</v>
       </c>
-      <c r="E3" s="27">
+      <c r="E3" s="26">
         <v>1.2585</v>
       </c>
-      <c r="F3" s="27">
+      <c r="F3" s="26">
         <v>1.1419999999999999</v>
       </c>
-      <c r="G3" s="27">
+      <c r="G3" s="26">
         <v>0.86170000000000002</v>
       </c>
     </row>
     <row r="4" spans="1:8" ht="15.6" x14ac:dyDescent="0.6">
-      <c r="A4" s="15" t="s">
+      <c r="A4" s="14" t="s">
         <v>10</v>
       </c>
-      <c r="B4" s="21">
+      <c r="B4" s="20">
         <v>10.4</v>
       </c>
-      <c r="C4" s="21">
+      <c r="C4" s="20">
         <v>17.48</v>
       </c>
-      <c r="D4" s="21">
+      <c r="D4" s="20">
         <v>15.36</v>
       </c>
-      <c r="E4" s="21">
+      <c r="E4" s="20">
         <v>44.3</v>
       </c>
-      <c r="F4" s="21">
+      <c r="F4" s="20">
         <v>97.86</v>
       </c>
-      <c r="G4" s="21">
+      <c r="G4" s="20">
         <v>104.12</v>
       </c>
     </row>
     <row r="5" spans="1:8" ht="15.6" x14ac:dyDescent="0.6">
-      <c r="A5" s="16" t="s">
+      <c r="A5" s="15" t="s">
         <v>11</v>
       </c>
-      <c r="B5" s="23">
+      <c r="B5" s="22">
         <v>0.62339999999999995</v>
       </c>
-      <c r="C5" s="23">
+      <c r="C5" s="22">
         <v>0.64929999999999999</v>
       </c>
-      <c r="D5" s="23">
+      <c r="D5" s="22">
         <v>0.56930000000000003</v>
       </c>
-      <c r="E5" s="23">
+      <c r="E5" s="22">
         <v>0.72719999999999996</v>
       </c>
-      <c r="F5" s="22">
+      <c r="F5" s="21">
         <v>0.74990000000000001</v>
       </c>
-      <c r="G5" s="22">
+      <c r="G5" s="21">
         <v>0.70109999999999995</v>
       </c>
-      <c r="H5" s="21"/>
+      <c r="H5" s="20"/>
     </row>
     <row r="6" spans="1:8" ht="15.6" x14ac:dyDescent="0.6">
-      <c r="A6" s="15" t="s">
+      <c r="A6" s="14" t="s">
         <v>12</v>
       </c>
-      <c r="B6" s="21">
+      <c r="B6" s="20">
         <v>4.53</v>
       </c>
-      <c r="C6" s="21">
+      <c r="C6" s="20">
         <v>10.039999999999999</v>
       </c>
-      <c r="D6" s="21">
+      <c r="D6" s="20">
         <v>5.58</v>
       </c>
-      <c r="E6" s="21">
+      <c r="E6" s="20">
         <v>32.97</v>
       </c>
-      <c r="F6" s="21">
+      <c r="F6" s="20">
         <v>81.45</v>
       </c>
-      <c r="G6" s="21">
+      <c r="G6" s="20">
         <v>86.18</v>
       </c>
     </row>
     <row r="7" spans="1:8" ht="15.6" x14ac:dyDescent="0.6">
-      <c r="A7" s="16" t="s">
+      <c r="A7" s="15" t="s">
         <v>13</v>
       </c>
-      <c r="B7" s="27">
+      <c r="B7" s="26">
         <v>0.27179999999999999</v>
       </c>
-      <c r="C7" s="27">
+      <c r="C7" s="26">
         <v>0.37309999999999999</v>
       </c>
-      <c r="D7" s="27">
+      <c r="D7" s="26">
         <v>0.20680000000000001</v>
       </c>
-      <c r="E7" s="27">
+      <c r="E7" s="26">
         <v>0.54120000000000001</v>
       </c>
-      <c r="F7" s="27">
+      <c r="F7" s="26">
         <v>0.62419999999999998</v>
       </c>
-      <c r="G7" s="27">
+      <c r="G7" s="26">
         <v>0.58030000000000004</v>
       </c>
     </row>
     <row r="8" spans="1:8" ht="15.6" x14ac:dyDescent="0.6">
-      <c r="A8" s="15" t="s">
+      <c r="A8" s="14" t="s">
         <v>14</v>
       </c>
-      <c r="B8" s="21">
+      <c r="B8" s="20">
         <v>4.54</v>
       </c>
-      <c r="C8" s="21">
+      <c r="C8" s="20">
         <v>10.15</v>
       </c>
-      <c r="D8" s="21">
+      <c r="D8" s="20">
         <v>4.18</v>
       </c>
-      <c r="E8" s="21">
+      <c r="E8" s="20">
         <v>33.21</v>
       </c>
-      <c r="F8" s="21">
+      <c r="F8" s="20">
         <v>82.49</v>
       </c>
-      <c r="G8" s="21">
+      <c r="G8" s="20">
         <v>86.96</v>
       </c>
     </row>
     <row r="9" spans="1:8" ht="15.6" x14ac:dyDescent="0.6">
-      <c r="A9" s="16" t="s">
+      <c r="A9" s="15" t="s">
         <v>15</v>
       </c>
-      <c r="B9" s="27">
+      <c r="B9" s="26">
         <v>0.27200000000000002</v>
       </c>
-      <c r="C9" s="27">
+      <c r="C9" s="26">
         <v>0.37709999999999999</v>
       </c>
-      <c r="D9" s="27">
+      <c r="D9" s="26">
         <v>0.15479999999999999</v>
       </c>
-      <c r="E9" s="27">
+      <c r="E9" s="26">
         <v>0.54510000000000003</v>
       </c>
-      <c r="F9" s="27">
+      <c r="F9" s="26">
         <v>0.6321</v>
       </c>
-      <c r="G9" s="27">
+      <c r="G9" s="26">
         <v>0.58550000000000002</v>
       </c>
     </row>
     <row r="10" spans="1:8" ht="15.6" x14ac:dyDescent="0.6">
-      <c r="A10" s="15" t="s">
+      <c r="A10" s="14" t="s">
         <v>16</v>
       </c>
-      <c r="B10" s="21">
+      <c r="B10" s="20">
         <v>5.63</v>
       </c>
-      <c r="C10" s="21">
+      <c r="C10" s="20">
         <v>11.32</v>
       </c>
-      <c r="D10" s="21">
+      <c r="D10" s="20">
         <v>5.72</v>
       </c>
-      <c r="E10" s="21">
+      <c r="E10" s="20">
         <v>34.72</v>
       </c>
-      <c r="F10" s="21">
+      <c r="F10" s="20">
         <v>84.38</v>
       </c>
-      <c r="G10" s="21">
+      <c r="G10" s="20">
         <v>89.03</v>
       </c>
     </row>
     <row r="11" spans="1:8" ht="15.6" x14ac:dyDescent="0.6">
-      <c r="A11" s="16" t="s">
+      <c r="A11" s="15" t="s">
         <v>17</v>
       </c>
-      <c r="B11" s="27">
+      <c r="B11" s="26">
         <v>0.33789999999999998</v>
       </c>
-      <c r="C11" s="27">
+      <c r="C11" s="26">
         <v>0.42070000000000002</v>
       </c>
-      <c r="D11" s="27">
+      <c r="D11" s="26">
         <v>0.21199999999999999</v>
       </c>
-      <c r="E11" s="27">
+      <c r="E11" s="26">
         <v>0.56989999999999996</v>
       </c>
-      <c r="F11" s="27">
+      <c r="F11" s="26">
         <v>0.64659999999999995</v>
       </c>
-      <c r="G11" s="27">
+      <c r="G11" s="26">
         <v>0.59940000000000004</v>
       </c>
     </row>
     <row r="12" spans="1:8" ht="15.6" x14ac:dyDescent="0.6">
-      <c r="A12" s="15" t="s">
+      <c r="A12" s="14" t="s">
         <v>18</v>
       </c>
-      <c r="B12" s="21">
+      <c r="B12" s="20">
         <v>4.33</v>
       </c>
-      <c r="C12" s="21">
+      <c r="C12" s="20">
         <v>9.75</v>
       </c>
-      <c r="D12" s="21">
+      <c r="D12" s="20">
         <v>4.37</v>
       </c>
-      <c r="E12" s="21">
+      <c r="E12" s="20">
         <v>29.76</v>
       </c>
-      <c r="F12" s="21">
+      <c r="F12" s="20">
         <v>72.88</v>
       </c>
-      <c r="G12" s="21">
+      <c r="G12" s="20">
         <v>76.77</v>
       </c>
     </row>
     <row r="13" spans="1:8" ht="15.6" x14ac:dyDescent="0.6">
-      <c r="A13" s="16" t="s">
+      <c r="A13" s="15" t="s">
         <v>19</v>
       </c>
-      <c r="B13" s="27">
+      <c r="B13" s="26">
         <v>0.25979999999999998</v>
       </c>
-      <c r="C13" s="27">
+      <c r="C13" s="26">
         <v>0.36230000000000001</v>
       </c>
-      <c r="D13" s="27">
+      <c r="D13" s="26">
         <v>0.16189999999999999</v>
       </c>
-      <c r="E13" s="27">
+      <c r="E13" s="26">
         <v>0.48849999999999999</v>
       </c>
-      <c r="F13" s="27">
+      <c r="F13" s="26">
         <v>0.5585</v>
       </c>
-      <c r="G13" s="27">
+      <c r="G13" s="26">
         <v>0.51690000000000003</v>
       </c>
     </row>
     <row r="14" spans="1:8" ht="15.6" x14ac:dyDescent="0.6">
-      <c r="A14" s="15" t="s">
+      <c r="A14" s="14" t="s">
         <v>20</v>
       </c>
-      <c r="B14" s="21">
+      <c r="B14" s="20">
         <v>0.18</v>
       </c>
-      <c r="C14" s="21">
+      <c r="C14" s="20">
         <v>0.39</v>
       </c>
-      <c r="D14" s="21">
+      <c r="D14" s="20">
         <v>0.18</v>
       </c>
-      <c r="E14" s="21">
+      <c r="E14" s="20">
         <v>1.21</v>
       </c>
-      <c r="F14" s="21">
+      <c r="F14" s="20">
         <v>2.97</v>
       </c>
-      <c r="G14" s="21">
+      <c r="G14" s="20">
         <v>3.14</v>
       </c>
     </row>
     <row r="15" spans="1:8" ht="15.6" x14ac:dyDescent="0.6">
-      <c r="A15" s="15" t="s">
+      <c r="A15" s="14" t="s">
         <v>21</v>
       </c>
-      <c r="B15" s="21">
+      <c r="B15" s="20">
         <v>0.17</v>
       </c>
-      <c r="C15" s="21">
+      <c r="C15" s="20">
         <v>0.39</v>
       </c>
-      <c r="D15" s="21">
+      <c r="D15" s="20">
         <v>0.17</v>
       </c>
-      <c r="E15" s="21">
+      <c r="E15" s="20">
         <v>1.19</v>
       </c>
-      <c r="F15" s="21">
+      <c r="F15" s="20">
         <v>2.94</v>
       </c>
-      <c r="G15" s="21">
+      <c r="G15" s="20">
         <v>3.1</v>
       </c>
     </row>
     <row r="16" spans="1:8" ht="15.6" x14ac:dyDescent="0.6">
-      <c r="A16" s="15" t="s">
+      <c r="A16" s="14" t="s">
         <v>22</v>
       </c>
-      <c r="B16" s="21">
+      <c r="B16" s="20">
         <v>0.25</v>
       </c>
-      <c r="C16" s="21">
+      <c r="C16" s="20">
         <v>0.44</v>
       </c>
-      <c r="D16" s="21">
+      <c r="D16" s="20">
         <v>0.33</v>
       </c>
-      <c r="E16" s="21">
+      <c r="E16" s="20">
         <v>1.3</v>
       </c>
-      <c r="F16" s="21">
+      <c r="F16" s="20">
         <v>2.99</v>
       </c>
-      <c r="G16" s="21">
+      <c r="G16" s="20">
         <v>3.19</v>
       </c>
     </row>
     <row r="17" spans="1:13" ht="15.6" x14ac:dyDescent="0.6">
-      <c r="A17" s="15" t="s">
+      <c r="A17" s="14" t="s">
         <v>23</v>
       </c>
-      <c r="B17" s="21">
+      <c r="B17" s="20">
         <v>0.02</v>
       </c>
-      <c r="C17" s="21">
+      <c r="C17" s="20">
         <v>0.02</v>
       </c>
-      <c r="D17" s="21">
+      <c r="D17" s="20">
         <v>0.02</v>
       </c>
-      <c r="E17" s="21">
+      <c r="E17" s="20">
         <v>0.02</v>
       </c>
-      <c r="F17" s="21">
+      <c r="F17" s="20">
         <v>0.03</v>
       </c>
-      <c r="G17" s="21">
+      <c r="G17" s="20">
         <v>0.04</v>
       </c>
     </row>
     <row r="18" spans="1:13" ht="15.6" x14ac:dyDescent="0.6">
-      <c r="A18" s="17"/>
-      <c r="B18" s="18"/>
-      <c r="C18" s="18"/>
-      <c r="D18" s="18"/>
-      <c r="E18" s="18"/>
-      <c r="F18" s="18"/>
-      <c r="G18" s="18"/>
+      <c r="A18" s="16"/>
+      <c r="B18" s="17"/>
+      <c r="C18" s="17"/>
+      <c r="D18" s="17"/>
+      <c r="E18" s="17"/>
+      <c r="F18" s="17"/>
+      <c r="G18" s="17"/>
     </row>
     <row r="19" spans="1:13" ht="15.6" x14ac:dyDescent="0.6">
       <c r="A19" s="12" t="s">
@@ -16449,226 +16651,226 @@
       </c>
     </row>
     <row r="20" spans="1:13" ht="15.6" x14ac:dyDescent="0.6">
-      <c r="A20" s="15" t="s">
+      <c r="A20" s="14" t="s">
         <v>26</v>
       </c>
-      <c r="B20" s="21">
+      <c r="B20" s="20">
         <v>28.79</v>
       </c>
-      <c r="C20" s="21">
+      <c r="C20" s="20">
         <v>44.19</v>
       </c>
-      <c r="D20" s="21">
+      <c r="D20" s="20">
         <v>41.18</v>
       </c>
-      <c r="E20" s="21">
+      <c r="E20" s="20">
         <v>65.73</v>
       </c>
-      <c r="F20" s="21">
+      <c r="F20" s="20">
         <v>111.6</v>
       </c>
-      <c r="G20" s="21">
+      <c r="G20" s="20">
         <v>125.25</v>
       </c>
     </row>
     <row r="21" spans="1:13" ht="15.6" x14ac:dyDescent="0.6">
-      <c r="A21" s="15" t="s">
+      <c r="A21" s="14" t="s">
         <v>27</v>
       </c>
-      <c r="B21" s="21">
+      <c r="B21" s="20">
         <v>11.9</v>
       </c>
-      <c r="C21" s="21">
+      <c r="C21" s="20">
         <v>17.579999999999998</v>
       </c>
-      <c r="D21" s="21">
+      <c r="D21" s="20">
         <v>19.079999999999998</v>
       </c>
-      <c r="E21" s="21">
+      <c r="E21" s="20">
         <v>22.75</v>
       </c>
-      <c r="F21" s="21">
+      <c r="F21" s="20">
         <v>32.270000000000003</v>
       </c>
-      <c r="G21" s="21">
+      <c r="G21" s="20">
         <v>41.41</v>
       </c>
     </row>
     <row r="22" spans="1:13" ht="15.6" x14ac:dyDescent="0.6">
-      <c r="A22" s="15" t="s">
+      <c r="A22" s="14" t="s">
         <v>28</v>
       </c>
-      <c r="B22" s="21">
+      <c r="B22" s="20">
         <v>7.72</v>
       </c>
-      <c r="C22" s="21">
+      <c r="C22" s="20">
         <v>11.69</v>
       </c>
-      <c r="D22" s="21">
+      <c r="D22" s="20">
         <v>12.03</v>
       </c>
-      <c r="E22" s="21">
+      <c r="E22" s="20">
         <v>11.06</v>
       </c>
-      <c r="F22" s="21">
+      <c r="F22" s="20">
         <v>10.27</v>
       </c>
-      <c r="G22" s="21">
+      <c r="G22" s="20">
         <v>10.29</v>
       </c>
     </row>
     <row r="23" spans="1:13" ht="15.6" x14ac:dyDescent="0.6">
-      <c r="A23" s="15" t="s">
+      <c r="A23" s="14" t="s">
         <v>29</v>
       </c>
-      <c r="B23" s="21">
+      <c r="B23" s="20">
         <v>16.89</v>
       </c>
-      <c r="C23" s="21">
+      <c r="C23" s="20">
         <v>26.61</v>
       </c>
-      <c r="D23" s="21">
+      <c r="D23" s="20">
         <v>22.1</v>
       </c>
-      <c r="E23" s="21">
+      <c r="E23" s="20">
         <v>42.98</v>
       </c>
-      <c r="F23" s="21">
+      <c r="F23" s="20">
         <v>79.33</v>
       </c>
-      <c r="G23" s="21">
+      <c r="G23" s="20">
         <v>83.84</v>
       </c>
     </row>
     <row r="24" spans="1:13" ht="15.6" x14ac:dyDescent="0.6">
-      <c r="A24" s="15" t="s">
+      <c r="A24" s="14" t="s">
         <v>30</v>
       </c>
-      <c r="B24" s="21">
+      <c r="B24" s="20">
         <v>0.85</v>
       </c>
-      <c r="C24" s="21">
+      <c r="C24" s="20">
         <v>1.99</v>
       </c>
-      <c r="D24" s="21">
+      <c r="D24" s="20">
         <v>3.39</v>
       </c>
-      <c r="E24" s="21">
+      <c r="E24" s="20">
         <v>7.28</v>
       </c>
-      <c r="F24" s="21">
+      <c r="F24" s="20">
         <v>8.59</v>
       </c>
-      <c r="G24" s="21">
+      <c r="G24" s="20">
         <v>15.23</v>
       </c>
     </row>
     <row r="25" spans="1:13" ht="15.6" x14ac:dyDescent="0.6">
-      <c r="A25" s="15" t="s">
+      <c r="A25" s="14" t="s">
         <v>31</v>
       </c>
-      <c r="B25" s="21">
+      <c r="B25" s="20">
         <v>12.13</v>
       </c>
-      <c r="C25" s="21">
+      <c r="C25" s="20">
         <v>24.49</v>
       </c>
-      <c r="D25" s="21">
+      <c r="D25" s="20">
         <v>16.510000000000002</v>
       </c>
-      <c r="E25" s="21">
+      <c r="E25" s="20">
         <v>33.71</v>
       </c>
-      <c r="F25" s="21">
+      <c r="F25" s="20">
         <v>62.08</v>
       </c>
-      <c r="G25" s="21">
+      <c r="G25" s="20">
         <v>63.39</v>
       </c>
-      <c r="H25" s="21"/>
-      <c r="I25" s="21"/>
-      <c r="J25" s="21"/>
-      <c r="K25" s="21"/>
-      <c r="L25" s="21"/>
-      <c r="M25" s="21"/>
+      <c r="H25" s="20"/>
+      <c r="I25" s="20"/>
+      <c r="J25" s="20"/>
+      <c r="K25" s="20"/>
+      <c r="L25" s="20"/>
+      <c r="M25" s="20"/>
     </row>
     <row r="26" spans="1:13" ht="15.6" x14ac:dyDescent="0.6">
-      <c r="A26" s="15" t="s">
+      <c r="A26" s="14" t="s">
         <v>32</v>
       </c>
-      <c r="B26" s="21">
+      <c r="B26" s="20">
         <v>25</v>
       </c>
-      <c r="C26" s="21">
+      <c r="C26" s="20">
         <v>24.6</v>
       </c>
-      <c r="D26" s="21">
+      <c r="D26" s="20">
         <v>24.7</v>
       </c>
-      <c r="E26" s="21">
+      <c r="E26" s="20">
         <v>24.49</v>
       </c>
-      <c r="F26" s="21">
+      <c r="F26" s="20">
         <v>24.39</v>
       </c>
-      <c r="G26" s="21">
+      <c r="G26" s="20">
         <v>24.39</v>
       </c>
     </row>
     <row r="27" spans="1:13" ht="15.6" x14ac:dyDescent="0.6">
-      <c r="A27" s="15" t="s">
+      <c r="A27" s="14" t="s">
         <v>33</v>
       </c>
-      <c r="B27" s="21">
+      <c r="B27" s="20">
         <v>0.68</v>
       </c>
-      <c r="C27" s="21">
+      <c r="C27" s="20">
         <v>1.06</v>
       </c>
-      <c r="D27" s="21">
+      <c r="D27" s="20">
         <v>0.9</v>
       </c>
-      <c r="E27" s="21">
+      <c r="E27" s="20">
         <v>1.74</v>
       </c>
-      <c r="F27" s="21">
+      <c r="F27" s="20">
         <v>3.24</v>
       </c>
-      <c r="G27" s="21">
+      <c r="G27" s="20">
         <v>3.44</v>
       </c>
     </row>
     <row r="28" spans="1:13" ht="15.6" x14ac:dyDescent="0.6">
-      <c r="A28" s="15" t="s">
+      <c r="A28" s="14" t="s">
         <v>34</v>
       </c>
-      <c r="B28" s="21">
+      <c r="B28" s="20">
         <v>0.46</v>
       </c>
-      <c r="C28" s="21">
+      <c r="C28" s="20">
         <v>0.44</v>
       </c>
-      <c r="D28" s="21">
+      <c r="D28" s="20">
         <v>0.54</v>
       </c>
-      <c r="E28" s="21">
+      <c r="E28" s="20">
         <v>0.26</v>
       </c>
-      <c r="F28" s="21">
+      <c r="F28" s="20">
         <v>0.13</v>
       </c>
-      <c r="G28" s="21">
+      <c r="G28" s="20">
         <v>0.12</v>
       </c>
     </row>
     <row r="29" spans="1:13" ht="15.6" x14ac:dyDescent="0.6">
-      <c r="A29" s="17"/>
-      <c r="B29" s="18"/>
-      <c r="C29" s="18"/>
-      <c r="D29" s="18"/>
-      <c r="E29" s="18"/>
-      <c r="F29" s="18"/>
-      <c r="G29" s="18"/>
+      <c r="A29" s="16"/>
+      <c r="B29" s="17"/>
+      <c r="C29" s="17"/>
+      <c r="D29" s="17"/>
+      <c r="E29" s="17"/>
+      <c r="F29" s="17"/>
+      <c r="G29" s="17"/>
     </row>
     <row r="30" spans="1:13" ht="31.2" x14ac:dyDescent="0.6">
       <c r="A30" s="12" t="s">
@@ -16694,140 +16896,140 @@
       </c>
     </row>
     <row r="31" spans="1:13" ht="15.6" x14ac:dyDescent="0.6">
-      <c r="A31" s="15" t="s">
+      <c r="A31" s="14" t="s">
         <v>36</v>
       </c>
-      <c r="B31" s="21">
+      <c r="B31" s="20">
         <v>5.82</v>
       </c>
-      <c r="C31" s="21">
+      <c r="C31" s="20">
         <v>9.11</v>
       </c>
-      <c r="D31" s="21">
+      <c r="D31" s="20">
         <v>5.64</v>
       </c>
-      <c r="E31" s="21">
+      <c r="E31" s="20">
         <v>28.09</v>
       </c>
-      <c r="F31" s="21">
+      <c r="F31" s="20">
         <v>64.09</v>
       </c>
-      <c r="G31" s="21">
+      <c r="G31" s="20">
         <v>76.16</v>
       </c>
     </row>
     <row r="32" spans="1:13" ht="15.6" x14ac:dyDescent="0.6">
-      <c r="A32" s="15" t="s">
+      <c r="A32" s="14" t="s">
         <v>37</v>
       </c>
-      <c r="B32" s="21">
+      <c r="B32" s="20">
         <v>-19.68</v>
       </c>
-      <c r="C32" s="21">
+      <c r="C32" s="20">
         <v>-9.83</v>
       </c>
-      <c r="D32" s="21">
+      <c r="D32" s="20">
         <v>7.38</v>
       </c>
-      <c r="E32" s="21">
+      <c r="E32" s="20">
         <v>-10.57</v>
       </c>
-      <c r="F32" s="21">
+      <c r="F32" s="20">
         <v>-20.420000000000002</v>
       </c>
-      <c r="G32" s="21">
+      <c r="G32" s="20">
         <v>-19.940000000000001</v>
       </c>
     </row>
     <row r="33" spans="1:7" ht="15.6" x14ac:dyDescent="0.6">
-      <c r="A33" s="15" t="s">
+      <c r="A33" s="14" t="s">
         <v>38</v>
       </c>
-      <c r="B33" s="21">
+      <c r="B33" s="20">
         <v>3.8</v>
       </c>
-      <c r="C33" s="21">
+      <c r="C33" s="20">
         <v>1.87</v>
       </c>
-      <c r="D33" s="21">
+      <c r="D33" s="20">
         <v>-11.62</v>
       </c>
-      <c r="E33" s="21">
+      <c r="E33" s="20">
         <v>-13.63</v>
       </c>
-      <c r="F33" s="21">
+      <c r="F33" s="20">
         <v>-42.36</v>
       </c>
-      <c r="G33" s="21">
+      <c r="G33" s="20">
         <v>-48.57</v>
       </c>
     </row>
     <row r="34" spans="1:7" ht="15.6" x14ac:dyDescent="0.6">
-      <c r="A34" s="15" t="s">
+      <c r="A34" s="14" t="s">
         <v>39</v>
       </c>
-      <c r="B34" s="21">
+      <c r="B34" s="20">
         <v>1.1299999999999999</v>
       </c>
-      <c r="C34" s="21">
+      <c r="C34" s="20">
         <v>0.98</v>
       </c>
-      <c r="D34" s="21">
+      <c r="D34" s="20">
         <v>1.83</v>
       </c>
-      <c r="E34" s="21">
+      <c r="E34" s="20">
         <v>1.07</v>
       </c>
-      <c r="F34" s="21">
+      <c r="F34" s="20">
         <v>3.24</v>
       </c>
-      <c r="G34" s="21">
+      <c r="G34" s="20">
         <v>4.09</v>
       </c>
     </row>
     <row r="35" spans="1:7" ht="15.6" x14ac:dyDescent="0.6">
-      <c r="A35" s="15" t="s">
+      <c r="A35" s="14" t="s">
         <v>40</v>
       </c>
-      <c r="B35" s="21">
+      <c r="B35" s="20">
         <v>5.4</v>
       </c>
-      <c r="C35" s="21">
+      <c r="C35" s="20">
         <v>11.5</v>
       </c>
-      <c r="D35" s="21">
+      <c r="D35" s="20">
         <v>6.01</v>
       </c>
-      <c r="E35" s="21">
+      <c r="E35" s="20">
         <v>30.74</v>
       </c>
-      <c r="F35" s="21">
+      <c r="F35" s="20">
         <v>70.239999999999995</v>
       </c>
-      <c r="G35" s="21">
+      <c r="G35" s="20">
         <v>73.63</v>
       </c>
     </row>
     <row r="36" spans="1:7" ht="15.6" x14ac:dyDescent="0.6">
-      <c r="A36" s="15" t="s">
+      <c r="A36" s="14" t="s">
         <v>41</v>
       </c>
-      <c r="B36" s="21">
+      <c r="B36" s="20">
         <v>-10.050000000000001</v>
       </c>
-      <c r="C36" s="21">
+      <c r="C36" s="20">
         <v>1.1399999999999999</v>
       </c>
-      <c r="D36" s="21">
+      <c r="D36" s="20">
         <v>1.4</v>
       </c>
-      <c r="E36" s="21">
+      <c r="E36" s="20">
         <v>3.89</v>
       </c>
-      <c r="F36" s="21">
+      <c r="F36" s="20">
         <v>1.31</v>
       </c>
-      <c r="G36" s="21">
+      <c r="G36" s="20">
         <v>7.65</v>
       </c>
     </row>

</xml_diff>